<commit_message>
Update Excel files to contain new value options
</commit_message>
<xml_diff>
--- a/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
+++ b/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
@@ -416,7 +416,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="427">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -1339,6 +1339,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000250</t>
   </si>
   <si>
+    <t>10X Genomics; Visium CytAssist Spatial Gene Expression for FFPE, Human Transcriptome, 11 mm, 2 reactions; PN 1000522</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000322</t>
+  </si>
+  <si>
     <t>10X Genomics; Visium Spatial Gene Expression Slide and Reagent Kit, 4 slides, 16 reactions; PN 1000184</t>
   </si>
   <si>
@@ -1357,6 +1363,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000260</t>
   </si>
   <si>
+    <t>10X Genomics; Visium Spatial for FFPE Gene Expression Kit, Human Transcriptome, 1 slides, 4 reactions; PN 1000338</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000320</t>
+  </si>
+  <si>
     <t>10X Genomics; Chromium Single Cell 3' Library &amp; Gel Bead Kit, 4 rxns; PN-120267</t>
   </si>
   <si>
@@ -1375,6 +1387,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000265</t>
   </si>
   <si>
+    <t>10X Genomics; Visium CytAssist Spatial Gene Expression for FFPE, Human Transcriptome, 6.5mm, 4 reactions; PN 1000520</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000321</t>
+  </si>
+  <si>
     <t>sample_indexing_kit</t>
   </si>
   <si>
@@ -1438,6 +1456,18 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000254</t>
   </si>
   <si>
+    <t>Illumina; NovaSeq 6000 S1 Reagent v1.5 Kit (300 Cycles); PN 20028317</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000318</t>
+  </si>
+  <si>
+    <t>Illumina; NextSeq 1000/2000 P2 Reagent v3 Kit (100 Cycles); PN 20046811</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000323</t>
+  </si>
+  <si>
     <t>Illumina; NovaSeq X Series 10B Reagent Kit (200 Cycle); PN 20085595</t>
   </si>
   <si>
@@ -1468,6 +1498,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000287</t>
   </si>
   <si>
+    <t>Illumina; NovaSeq 6000 S4 Reagent Kit v1.5 (300 cycles); PN 20028312</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000319</t>
+  </si>
+  <si>
     <t>Illumina; NovaSeq X Series 10B Reagent Kit (300 Cycle); PN 20085594</t>
   </si>
   <si>
@@ -1582,6 +1618,18 @@
     <t>preparation_instrument_kit</t>
   </si>
   <si>
+    <t>10X Genomics; Visium FFPE Reagent Kit v2-Small, PN 1000436</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000324</t>
+  </si>
+  <si>
+    <t>10x Genomics; Chromium Next GEM Chip Q Single Cell Kit, 16 rxns; PN 1000422</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000325</t>
+  </si>
+  <si>
     <t>probe_hybridization_time_value</t>
   </si>
   <si>
@@ -1615,6 +1663,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000274</t>
   </si>
   <si>
+    <t>10x Genomics; Visium Human Transcriptome Probe Kit-Small; PN 1000363</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000326</t>
+  </si>
+  <si>
     <t>is_custom_probes_used</t>
   </si>
   <si>
@@ -1636,7 +1690,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-01-29T14:35:01-08:00</t>
+    <t>2024-02-08T09:17:07-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1932,52 +1986,52 @@
         <v>304</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="AO1" t="s" s="1">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="AP1" t="s" s="1">
-        <v>356</v>
+        <v>368</v>
       </c>
       <c r="AQ1" t="s" s="1">
-        <v>357</v>
+        <v>369</v>
       </c>
       <c r="AR1" t="s" s="1">
-        <v>358</v>
+        <v>370</v>
       </c>
       <c r="AS1" t="s" s="1">
-        <v>359</v>
+        <v>371</v>
       </c>
       <c r="AT1" t="s" s="1">
-        <v>366</v>
+        <v>378</v>
       </c>
       <c r="AU1" t="s" s="1">
-        <v>387</v>
+        <v>399</v>
       </c>
       <c r="AV1" t="s" s="1">
-        <v>388</v>
+        <v>404</v>
       </c>
       <c r="AW1" t="s" s="1">
-        <v>389</v>
+        <v>405</v>
       </c>
       <c r="AX1" t="s" s="1">
-        <v>390</v>
+        <v>406</v>
       </c>
       <c r="AY1" t="s" s="1">
-        <v>399</v>
+        <v>417</v>
       </c>
       <c r="AZ1" t="s" s="1">
-        <v>400</v>
+        <v>418</v>
       </c>
     </row>
     <row r="2">
@@ -1985,7 +2039,7 @@
         <v>62</v>
       </c>
       <c r="AZ2" t="s" s="53">
-        <v>401</v>
+        <v>419</v>
       </c>
     </row>
   </sheetData>
@@ -2088,7 +2142,7 @@
       <formula2>2147483647</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="AJ2:AJ1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'library_preparation_kit'!$A$1:$A$7</formula1>
+      <formula1>'library_preparation_kit'!$A$1:$A$10</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AK2:AK1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'sample_indexing_kit'!$A$1:$A$4</formula1>
@@ -2101,7 +2155,7 @@
       <formula2>2147483647</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="AO2:AO1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'sequencing_reagent_kit'!$A$1:$A$13</formula1>
+      <formula1>'sequencing_reagent_kit'!$A$1:$A$16</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AS2:AS1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'preparation_instrument_vendor'!$A$1:$A$7</formula1>
@@ -2110,7 +2164,7 @@
       <formula1>'preparation_instrument_model'!$A$1:$A$14</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AU2:AU1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_instrument_kit'!$A$1:$A$2</formula1>
+      <formula1>'preparation_instrument_kit'!$A$1:$A$4</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="between" sqref="AV2:AV1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be a number" showErrorMessage="true">
       <formula1>-3.4028235E38</formula1>
@@ -2120,7 +2174,7 @@
       <formula1>'probe_hybridization_time_unit'!$A$1:$A$1</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AX2:AX1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'oligo_probe_panel'!$A$1:$A$5</formula1>
+      <formula1>'oligo_probe_panel'!$A$1:$A$6</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AY2:AY1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_custom_probes_used'!$A$1:$A$2</formula1>
@@ -2768,7 +2822,7 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2828,6 +2882,30 @@
       </c>
       <c r="B7" t="s" s="0">
         <v>318</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>319</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>321</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>323</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -2845,10 +2923,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>321</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2">
@@ -2861,18 +2939,18 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>323</v>
+        <v>329</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>325</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -2905,7 +2983,7 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2913,106 +2991,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>331</v>
+        <v>337</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>332</v>
+        <v>338</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>333</v>
+        <v>339</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>335</v>
+        <v>341</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>337</v>
+        <v>343</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>338</v>
+        <v>344</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>339</v>
+        <v>345</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>341</v>
+        <v>347</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>342</v>
+        <v>348</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>343</v>
+        <v>349</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>344</v>
+        <v>350</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>345</v>
+        <v>351</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>346</v>
+        <v>352</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>347</v>
+        <v>353</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>348</v>
+        <v>354</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>349</v>
+        <v>355</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>350</v>
+        <v>356</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>351</v>
+        <v>357</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>353</v>
+        <v>359</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>354</v>
+        <v>360</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>355</v>
+        <v>361</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>362</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>364</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>366</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>367</v>
       </c>
     </row>
   </sheetData>
@@ -3054,18 +3156,18 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>360</v>
+        <v>372</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>361</v>
+        <v>373</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>362</v>
+        <v>374</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>363</v>
+        <v>375</v>
       </c>
     </row>
     <row r="6">
@@ -3078,10 +3180,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>365</v>
+        <v>377</v>
       </c>
     </row>
   </sheetData>
@@ -3115,18 +3217,18 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>367</v>
+        <v>379</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>368</v>
+        <v>380</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>369</v>
+        <v>381</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>370</v>
+        <v>382</v>
       </c>
     </row>
     <row r="5">
@@ -3147,66 +3249,66 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>371</v>
+        <v>383</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>372</v>
+        <v>384</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>373</v>
+        <v>385</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>374</v>
+        <v>386</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>375</v>
+        <v>387</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>376</v>
+        <v>388</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>377</v>
+        <v>389</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>378</v>
+        <v>390</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>379</v>
+        <v>391</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>380</v>
+        <v>392</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>381</v>
+        <v>393</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>382</v>
+        <v>394</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>383</v>
+        <v>395</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>384</v>
+        <v>396</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>385</v>
+        <v>397</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>386</v>
+        <v>398</v>
       </c>
     </row>
   </sheetData>
@@ -3216,7 +3318,7 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3224,10 +3326,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="2">
@@ -3236,6 +3338,22 @@
       </c>
       <c r="B2" t="s" s="0">
         <v>306</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>400</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>402</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>403</v>
       </c>
     </row>
   </sheetData>
@@ -3266,7 +3384,7 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3274,42 +3392,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>391</v>
+        <v>407</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>392</v>
+        <v>408</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>393</v>
+        <v>409</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>394</v>
+        <v>410</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>316</v>
+        <v>320</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>395</v>
+        <v>411</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>396</v>
+        <v>412</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>397</v>
+        <v>413</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>398</v>
+        <v>414</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>415</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>416</v>
       </c>
     </row>
   </sheetData>
@@ -3457,16 +3583,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>402</v>
+        <v>420</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>403</v>
+        <v>421</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>405</v>
+        <v>423</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>407</v>
+        <v>425</v>
       </c>
     </row>
     <row r="2">
@@ -3474,13 +3600,13 @@
         <v>62</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>404</v>
+        <v>422</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>406</v>
+        <v>424</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>408</v>
+        <v>426</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Excel files with a new vendor and model
</commit_message>
<xml_diff>
--- a/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
+++ b/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
@@ -416,7 +416,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="431">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -805,6 +805,12 @@
     <t>https://identifiers.org/RRID:SCR_023609</t>
   </si>
   <si>
+    <t>Huron Digital Pathology</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024996</t>
+  </si>
+  <si>
     <t>Illumina</t>
   </si>
   <si>
@@ -934,6 +940,12 @@
     <t>https://identifiers.org/RRID:SCR_023615</t>
   </si>
   <si>
+    <t>TissueScope LE Slide Scanner</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024995</t>
+  </si>
+  <si>
     <t>VS200 Slide Scanner</t>
   </si>
   <si>
@@ -1690,7 +1702,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-02-08T09:17:07-08:00</t>
+    <t>2024-02-09T10:29:34-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1899,139 +1911,139 @@
         <v>96</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="AO1" t="s" s="1">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="AP1" t="s" s="1">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="AQ1" t="s" s="1">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="AR1" t="s" s="1">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="AS1" t="s" s="1">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="AT1" t="s" s="1">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="AU1" t="s" s="1">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="AV1" t="s" s="1">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="AW1" t="s" s="1">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="AX1" t="s" s="1">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="AY1" t="s" s="1">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="AZ1" t="s" s="1">
-        <v>418</v>
+        <v>422</v>
       </c>
     </row>
     <row r="2">
@@ -2039,7 +2051,7 @@
         <v>62</v>
       </c>
       <c r="AZ2" t="s" s="53">
-        <v>419</v>
+        <v>423</v>
       </c>
     </row>
   </sheetData>
@@ -2054,10 +2066,10 @@
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$19</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$20</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$45</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$46</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -2196,26 +2208,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>252</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>254</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -2233,32 +2245,32 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>257</v>
+        <v>261</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>258</v>
+        <v>262</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>260</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -2276,17 +2288,17 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>258</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -2304,26 +2316,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>252</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>254</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -2341,27 +2353,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>264</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>266</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -2379,42 +2391,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>275</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -2432,10 +2444,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>282</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -2453,10 +2465,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>288</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -2474,10 +2486,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>288</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -2495,18 +2507,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>294</v>
+        <v>298</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -2801,18 +2813,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>299</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>301</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -2830,82 +2842,82 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>306</v>
+        <v>310</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>308</v>
+        <v>312</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>310</v>
+        <v>314</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>312</v>
+        <v>316</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>314</v>
+        <v>318</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>316</v>
+        <v>320</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>318</v>
+        <v>322</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>320</v>
+        <v>324</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>322</v>
+        <v>326</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>324</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -2923,34 +2935,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>327</v>
+        <v>331</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>252</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>329</v>
+        <v>333</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>331</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>
@@ -2991,130 +3003,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>337</v>
+        <v>341</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>339</v>
+        <v>343</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>341</v>
+        <v>345</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>343</v>
+        <v>347</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>345</v>
+        <v>349</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>347</v>
+        <v>351</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>349</v>
+        <v>353</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>351</v>
+        <v>355</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>353</v>
+        <v>357</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>355</v>
+        <v>359</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>357</v>
+        <v>361</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>359</v>
+        <v>363</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>361</v>
+        <v>365</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>363</v>
+        <v>367</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>365</v>
+        <v>369</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>367</v>
+        <v>371</v>
       </c>
     </row>
   </sheetData>
@@ -3148,26 +3160,26 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>252</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>373</v>
+        <v>377</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>375</v>
+        <v>379</v>
       </c>
     </row>
     <row r="6">
@@ -3180,10 +3192,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>377</v>
+        <v>381</v>
       </c>
     </row>
   </sheetData>
@@ -3201,114 +3213,114 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>252</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>380</v>
+        <v>384</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>382</v>
+        <v>386</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>384</v>
+        <v>388</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>386</v>
+        <v>390</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>388</v>
+        <v>392</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>390</v>
+        <v>394</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>392</v>
+        <v>396</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>394</v>
+        <v>398</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>396</v>
+        <v>400</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>398</v>
+        <v>402</v>
       </c>
     </row>
   </sheetData>
@@ -3326,34 +3338,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>312</v>
+        <v>316</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>306</v>
+        <v>310</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>401</v>
+        <v>405</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>403</v>
+        <v>407</v>
       </c>
     </row>
   </sheetData>
@@ -3371,10 +3383,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -3392,50 +3404,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>408</v>
+        <v>412</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>410</v>
+        <v>414</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>320</v>
+        <v>324</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>412</v>
+        <v>416</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>414</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>416</v>
+        <v>420</v>
       </c>
     </row>
   </sheetData>
@@ -3583,16 +3595,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>425</v>
+        <v>429</v>
       </c>
     </row>
     <row r="2">
@@ -3600,13 +3612,13 @@
         <v>62</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>426</v>
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -3639,7 +3651,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3797,6 +3809,14 @@
         <v>134</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>135</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>136</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -3804,7 +3824,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3812,362 +3832,370 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>225</v>
+        <v>227</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>228</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -4185,42 +4213,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>231</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>233</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>235</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -4238,26 +4266,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>231</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>233</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>235</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -4275,32 +4303,32 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>244</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update RNAseq spreadsheet files
</commit_message>
<xml_diff>
--- a/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
+++ b/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
@@ -416,7 +416,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="431">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -1273,10 +1273,16 @@
     <t>amount_of_input_analyte_unit</t>
   </si>
   <si>
-    <t>Amount of input analyte unit</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_1001221</t>
+    <t>ng</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000024</t>
+  </si>
+  <si>
+    <t>ug</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000023</t>
   </si>
   <si>
     <t>library_adapter_sequence</t>
@@ -1291,12 +1297,6 @@
     <t>library_input_amount_unit</t>
   </si>
   <si>
-    <t>ng</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/UO_0000024</t>
-  </si>
-  <si>
     <t>library_output_amount_value</t>
   </si>
   <si>
@@ -1702,7 +1702,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-02-09T10:29:34-08:00</t>
+    <t>2024-02-13T14:42:31-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1962,16 +1962,16 @@
         <v>284</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="AC1" t="s" s="1">
         <v>293</v>
@@ -2115,7 +2115,7 @@
       <formula2>3.4028235E38</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="X2:X1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'amount_of_input_analyte_unit'!$A$1:$A$1</formula1>
+      <formula1>'amount_of_input_analyte_unit'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="between" sqref="Z2:Z1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be a number" showErrorMessage="true">
       <formula1>-2147483648</formula1>
@@ -2436,7 +2436,7 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2448,6 +2448,14 @@
       </c>
       <c r="B1" t="s" s="0">
         <v>286</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>287</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -2465,10 +2473,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>292</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -2486,10 +2494,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>292</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the probe hybridization definition and add 'hour' in the time unit
Closes #5
</commit_message>
<xml_diff>
--- a/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
+++ b/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
@@ -380,8 +380,8 @@
     </comment>
     <comment ref="AV1" authorId="1">
       <text>
-        <t>(Required) How many hours were the oligo-conjugated RNA or oligo-conjugated
-antibody probes hybridized with the sample?</t>
+        <t>(Required) How long was the oligo-conjugated RNA or oligo-conjugated antibody
+probes hybridized with the sample?</t>
       </text>
     </comment>
     <comment ref="AW1" authorId="1">
@@ -416,7 +416,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="437">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -880,6 +880,12 @@
     <t>https://identifiers.org/RRID:SCR_023616</t>
   </si>
   <si>
+    <t>PhenoImager Fusion</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023274</t>
+  </si>
+  <si>
     <t>DM6 B</t>
   </si>
   <si>
@@ -1030,6 +1036,12 @@
     <t>https://identifiers.org/RRID:SCR_023617</t>
   </si>
   <si>
+    <t>Aperio AT2</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_021256</t>
+  </si>
+  <si>
     <t>MIBIscope</t>
   </si>
   <si>
@@ -1609,6 +1621,12 @@
     <t>https://identifiers.org/RRID:SCR_023731</t>
   </si>
   <si>
+    <t>ST5020 Multistainer</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_025021</t>
+  </si>
+  <si>
     <t>Chromium iX</t>
   </si>
   <si>
@@ -1702,7 +1720,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-02-13T14:42:31-08:00</t>
+    <t>2024-02-29T07:10:17-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1914,136 +1932,136 @@
         <v>137</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="AO1" t="s" s="1">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="AP1" t="s" s="1">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="AQ1" t="s" s="1">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="AR1" t="s" s="1">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="AS1" t="s" s="1">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="AT1" t="s" s="1">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="AU1" t="s" s="1">
-        <v>403</v>
+        <v>409</v>
       </c>
       <c r="AV1" t="s" s="1">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="AW1" t="s" s="1">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="AX1" t="s" s="1">
-        <v>410</v>
+        <v>416</v>
       </c>
       <c r="AY1" t="s" s="1">
-        <v>421</v>
+        <v>427</v>
       </c>
       <c r="AZ1" t="s" s="1">
-        <v>422</v>
+        <v>428</v>
       </c>
     </row>
     <row r="2">
@@ -2051,7 +2069,7 @@
         <v>62</v>
       </c>
       <c r="AZ2" t="s" s="53">
-        <v>423</v>
+        <v>429</v>
       </c>
     </row>
   </sheetData>
@@ -2069,7 +2087,7 @@
       <formula1>'acquisition_instrument_vendor'!$A$1:$A$20</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$46</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$48</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -2173,7 +2191,7 @@
       <formula1>'preparation_instrument_vendor'!$A$1:$A$7</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AT2:AT1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_instrument_model'!$A$1:$A$14</formula1>
+      <formula1>'preparation_instrument_model'!$A$1:$A$15</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AU2:AU1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'preparation_instrument_kit'!$A$1:$A$4</formula1>
@@ -2183,7 +2201,7 @@
       <formula2>3.4028235E38</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="AW2:AW1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'probe_hybridization_time_unit'!$A$1:$A$1</formula1>
+      <formula1>'probe_hybridization_time_unit'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AX2:AX1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'oligo_probe_panel'!$A$1:$A$6</formula1>
@@ -2208,26 +2226,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>258</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -2245,32 +2263,32 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>260</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>262</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>264</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -2288,17 +2306,17 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>262</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -2316,26 +2334,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>258</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -2353,27 +2371,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>270</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -2391,42 +2409,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>275</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>279</v>
+        <v>283</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>281</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -2444,18 +2462,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>288</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -2473,10 +2491,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -2494,10 +2512,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -2515,18 +2533,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>298</v>
+        <v>302</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>300</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -2821,18 +2839,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>303</v>
+        <v>307</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>305</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -2850,82 +2868,82 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>310</v>
+        <v>314</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>312</v>
+        <v>316</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>314</v>
+        <v>318</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>316</v>
+        <v>320</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>318</v>
+        <v>322</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>320</v>
+        <v>324</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>322</v>
+        <v>326</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>324</v>
+        <v>328</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>326</v>
+        <v>330</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>328</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -2943,34 +2961,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>331</v>
+        <v>335</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>333</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>335</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -3011,130 +3029,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>341</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>343</v>
+        <v>347</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>345</v>
+        <v>349</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>347</v>
+        <v>351</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>349</v>
+        <v>353</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>351</v>
+        <v>355</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>353</v>
+        <v>357</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>355</v>
+        <v>359</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>357</v>
+        <v>361</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>359</v>
+        <v>363</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>361</v>
+        <v>365</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>363</v>
+        <v>367</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>365</v>
+        <v>369</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>367</v>
+        <v>371</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>369</v>
+        <v>373</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>371</v>
+        <v>375</v>
       </c>
     </row>
   </sheetData>
@@ -3168,26 +3186,26 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>377</v>
+        <v>381</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>379</v>
+        <v>383</v>
       </c>
     </row>
     <row r="6">
@@ -3200,10 +3218,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>381</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>
@@ -3213,7 +3231,7 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3229,106 +3247,114 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>384</v>
+        <v>388</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>386</v>
+        <v>390</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>388</v>
+        <v>392</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>390</v>
+        <v>394</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>392</v>
+        <v>396</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>394</v>
+        <v>398</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>396</v>
+        <v>400</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>398</v>
+        <v>402</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>402</v>
+        <v>406</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>407</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>408</v>
       </c>
     </row>
   </sheetData>
@@ -3346,34 +3372,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>316</v>
+        <v>320</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>310</v>
+        <v>314</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>404</v>
+        <v>410</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>405</v>
+        <v>411</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>406</v>
+        <v>412</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>407</v>
+        <v>413</v>
       </c>
     </row>
   </sheetData>
@@ -3383,7 +3409,7 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3391,10 +3417,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>241</v>
+        <v>237</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>244</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -3412,50 +3446,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>411</v>
+        <v>417</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>412</v>
+        <v>418</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>413</v>
+        <v>419</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>414</v>
+        <v>420</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>324</v>
+        <v>328</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>415</v>
+        <v>421</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>416</v>
+        <v>422</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>417</v>
+        <v>423</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>418</v>
+        <v>424</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>419</v>
+        <v>425</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>420</v>
+        <v>426</v>
       </c>
     </row>
   </sheetData>
@@ -3603,16 +3637,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>427</v>
+        <v>433</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>429</v>
+        <v>435</v>
       </c>
     </row>
     <row r="2">
@@ -3620,13 +3654,13 @@
         <v>62</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>428</v>
+        <v>434</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>430</v>
+        <v>436</v>
       </c>
     </row>
   </sheetData>
@@ -3832,7 +3866,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4204,6 +4238,22 @@
       </c>
       <c r="B46" t="s" s="0">
         <v>229</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>230</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>232</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -4221,42 +4271,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>233</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>235</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>239</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>241</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -4274,26 +4324,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>235</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>239</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -4311,32 +4361,32 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>250</v>
+        <v>254</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>252</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new preparation, indexing, reagent, and oligo kits
Closes #12, #13, #14
</commit_message>
<xml_diff>
--- a/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
+++ b/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
@@ -416,7 +416,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="513">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -751,6 +751,12 @@
     <t>https://identifiers.org/RRID:SCR_008452</t>
   </si>
   <si>
+    <t>Roche Diagnostics</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_025096</t>
+  </si>
+  <si>
     <t>Zeiss Microscopy</t>
   </si>
   <si>
@@ -910,6 +916,12 @@
     <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C17998</t>
   </si>
   <si>
+    <t>Discovery Ultra</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_025097</t>
+  </si>
+  <si>
     <t>Q Exactive UHMR</t>
   </si>
   <si>
@@ -1387,6 +1399,90 @@
     <t>library_preparation_kit</t>
   </si>
   <si>
+    <t>10X Genomics; Chromium Next GEM Single Cell 3' HT Kit v3.1, 8 rxns; PN 1000370</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000336</t>
+  </si>
+  <si>
+    <t>Illumina; TruSeq Stranded mRNA Library Prep (96 samples); PN 20020595</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000344</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium Next GEM Single Cell 5' Kit v2, 4 rxns; PN 1000265</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000340</t>
+  </si>
+  <si>
+    <t>10X Genomics; Visium Spatial Gene Expression Slide and Reagent Kit, 4 slides, 16 reactions; PN 1000184</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000261</t>
+  </si>
+  <si>
+    <t>Parse Biosciences; Evercode WT v2 Kit, 48 rxns; PN ECW02030</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000341</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium NextGem Single Cell Multiome ATAC + Gene Expression Reagent Bundle, 4 rxn; PN 1000285</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000251</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium Next GEM Single Cell 5' Kit v2, 16 rxns; PN 1000263</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000339</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium Single Cell 3' GEM, Library &amp; Gel Bead Kit v3, 4 rxns PN 1000092</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000260</t>
+  </si>
+  <si>
+    <t>10X Genomics; Visium Spatial for FFPE Gene Expression Kit, Human Transcriptome, 1 slides, 4 reactions; PN 1000338</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000320</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium Next GEM Single Cell 3' Kit v3.1, 16 rxns; PN 1000268</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000337</t>
+  </si>
+  <si>
+    <t>Custom</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C65167</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium Next GEM Single Cell 3' HT Kit v3.1, 48 rxns; PN 1000348</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000335</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium Single Cell 3' Library &amp; Gel Bead Kit, 4 rxns; PN 120267</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000299</t>
+  </si>
+  <si>
+    <t>10X Genomics; Visium Spatial for FFPE Gene Expression Kit, Mouse Transcriptome, 4 rxns; PN 1000339</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000355</t>
+  </si>
+  <si>
     <t>10X Genomics; Chromium NextGem Single Cell Multiome ATAC + Gene Expression Reagent Bundle, 16 rxn; PN 1000283</t>
   </si>
   <si>
@@ -1399,40 +1495,22 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000322</t>
   </si>
   <si>
-    <t>10X Genomics; Visium Spatial Gene Expression Slide and Reagent Kit, 4 slides, 16 reactions; PN 1000184</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000261</t>
-  </si>
-  <si>
-    <t>10X Genomics; Chromium NextGem Single Cell Multiome ATAC + Gene Expression Reagent Bundle, 4 rxn; PN 1000285</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000251</t>
-  </si>
-  <si>
-    <t>10X Genomics; Chromium Single Cell 3' GEM, Library &amp; Gel Bead Kit v3, 4 rxns PN 1000092</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000260</t>
-  </si>
-  <si>
-    <t>10X Genomics; Visium Spatial for FFPE Gene Expression Kit, Human Transcriptome, 1 slides, 4 reactions; PN 1000338</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000320</t>
-  </si>
-  <si>
-    <t>10X Genomics; Chromium Single Cell 3' Library &amp; Gel Bead Kit, 4 rxns; PN-120267</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000299</t>
-  </si>
-  <si>
-    <t>Custom</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C65167</t>
+    <t>Illumina; TruSeq Stranded mRNA Library Prep (48 samples); PN 20020594</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000343</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium Next GEM Single Cell 3' Kit v3.1, 4 rxns; PN 1000269</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000338</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium Next GEM Single Cell 3’ GEM, Library &amp; Gel Bead Kit v3.1, 16 rxns; PN 1000121</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000334</t>
   </si>
   <si>
     <t>10X Genomics; Visium Spatial Gene Expression Slide and Reagent Kit, 1 slides, 4 reactions; PN 1000187</t>
@@ -1441,6 +1519,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000265</t>
   </si>
   <si>
+    <t>Parse Biosciences; Evercode WT Mini v2 Kit, 12 rxns; PN ECW02010</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000342</t>
+  </si>
+  <si>
     <t>10X Genomics; Visium CytAssist Spatial Gene Expression for FFPE, Human Transcriptome, 6.5mm, 4 reactions; PN 1000520</t>
   </si>
   <si>
@@ -1450,12 +1534,78 @@
     <t>sample_indexing_kit</t>
   </si>
   <si>
+    <t>Illumina; TruSeq RNA CD Index Plate (96 Indexes, 96 Samples); PN 20019792</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000349</t>
+  </si>
+  <si>
+    <t>Illumina; TruSeq RNA Single Indexes Set A (12 Indexes, 48 Samples); PN 20020492</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000347</t>
+  </si>
+  <si>
+    <t>Illumina; TruSeq RNA Single Indexes Set B (12 Indexes, 48 Samples); PN 20020493</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000348</t>
+  </si>
+  <si>
+    <t>NanoString Technologies; GeoMx Seq Code Pack; PN GMX-NGS-SEQ-AB</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000356</t>
+  </si>
+  <si>
+    <t>NanoString Technologies; GeoMx Seq Code Pack; PN GMX-NGS-SEQ-CD</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000357</t>
+  </si>
+  <si>
+    <t>NanoString Technologies; GeoMx Seq Code Pack; PN GMX-NGS-SEQ-EF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000358</t>
+  </si>
+  <si>
+    <t>NanoString Technologies; GeoMx Seq Code Pack; PN GMX-NGS-SEQ-GH</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000359</t>
+  </si>
+  <si>
+    <t>Parse Biosciences; Fragmentation Reagents; PN WX100</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000345</t>
+  </si>
+  <si>
+    <t>Integrated DNA Technologies: Custom DNA Oligos</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000351</t>
+  </si>
+  <si>
+    <t>Parse Biosciences; UDI Plate - WT; PN UDI1001</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000346</t>
+  </si>
+  <si>
     <t>10X Genomics; Dual Index Kit TS, Set A; PN 1000251</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000282</t>
   </si>
   <si>
+    <t>Illumina; IDT for Illumina - TruSeq RNA UD Indexes v2 (96 Indexes, 96 Samples); PN 20040871</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000350</t>
+  </si>
+  <si>
     <t>10X Genomics; Single Index Kit N, Set A (96 rxn); PN 1000212</t>
   </si>
   <si>
@@ -1492,6 +1642,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000288</t>
   </si>
   <si>
+    <t>Illumina; NovaSeq 6000 S1 Reagent v1.5 Kit (200 Cycles); PN 20028318</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000360</t>
+  </si>
+  <si>
     <t>Illumina; NovaSeq 6000 S1 Reagent v1.5 Kit (100 Cycles); PN 20028319</t>
   </si>
   <si>
@@ -1510,6 +1666,18 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000254</t>
   </si>
   <si>
+    <t>Illumina; NextSeq 1000/2000 P2 Reagent v3 Kit (300 Cycles); PN 20046813</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000353</t>
+  </si>
+  <si>
+    <t>Illumina; NextSeq 2000 P3 Reagents Kit (100 Cycles); PN 20040559</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000361</t>
+  </si>
+  <si>
     <t>Illumina; NovaSeq 6000 S1 Reagent v1.5 Kit (300 Cycles); PN 20028317</t>
   </si>
   <si>
@@ -1522,12 +1690,24 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000323</t>
   </si>
   <si>
+    <t>Illumina; NextSeq 2000 P3 Reagent Kit (300 Cycles); PN 20040561</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000354</t>
+  </si>
+  <si>
     <t>Illumina; NovaSeq X Series 10B Reagent Kit (200 Cycle); PN 20085595</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000284</t>
   </si>
   <si>
+    <t>Illumina; NextSeq 1000/2000 P2 Reagent v3 Kit (200 Cycles); PN 20046812</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000352</t>
+  </si>
+  <si>
     <t>Illumina; NextSeq 500/550 Hi Output Kit 150 Cycles; v2.5; PN 20024907</t>
   </si>
   <si>
@@ -1699,16 +1879,40 @@
     <t>oligo_probe_panel</t>
   </si>
   <si>
+    <t>10x Genomics; Chromium Fixed RNA Kit, Human Transcriptome 4 rxns x 16 BC; PN 1000476</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000308</t>
+  </si>
+  <si>
+    <t>NanoString Technologies; GeoMx Mouse Whole Transcriptome Atlas, 4 slides; PN GMX-RNA-NGS-MsWTA-4</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000364</t>
+  </si>
+  <si>
+    <t>10x Genomics; Visium Human Transcriptome Probe Kit-Small; PN 1000363</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000326</t>
+  </si>
+  <si>
     <t>10x Genomics; Chromium Fixed RNA Kit, Human Transcriptome, 4 rxns x 1 BC; PN 1000474</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000306</t>
   </si>
   <si>
-    <t>10x Genomics; Chromium Fixed RNA Kit, Human Transcriptome 4 rxns x 16 BC; PN 1000476</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000308</t>
+    <t>10x Genomics; Visium Mouse Transcriptome Probe Kit - Small; PN 1000365</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000362</t>
+  </si>
+  <si>
+    <t>NanoString Technologies; GeoMx Human Whole Transcriptome Atlas, 4 slides; PN GMX-RNA-NGS-HuWTA-4</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000363</t>
   </si>
   <si>
     <t>10x Genomics; Chromium Fixed RNA Kit, Human Transcriptome 4 rxns x 4 BC; PN 1000475</t>
@@ -1723,12 +1927,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000274</t>
   </si>
   <si>
-    <t>10x Genomics; Visium Human Transcriptome Probe Kit-Small; PN 1000363</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000326</t>
-  </si>
-  <si>
     <t>is_custom_probes_used</t>
   </si>
   <si>
@@ -1750,7 +1948,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-03-05T18:57:27-08:00</t>
+    <t>2024-03-18T09:18:02-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1959,139 +2157,139 @@
         <v>100</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>343</v>
+        <v>371</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>350</v>
+        <v>400</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>351</v>
+        <v>401</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>352</v>
+        <v>402</v>
       </c>
       <c r="AO1" t="s" s="1">
-        <v>353</v>
+        <v>403</v>
       </c>
       <c r="AP1" t="s" s="1">
-        <v>386</v>
+        <v>446</v>
       </c>
       <c r="AQ1" t="s" s="1">
-        <v>387</v>
+        <v>447</v>
       </c>
       <c r="AR1" t="s" s="1">
-        <v>388</v>
+        <v>448</v>
       </c>
       <c r="AS1" t="s" s="1">
-        <v>389</v>
+        <v>449</v>
       </c>
       <c r="AT1" t="s" s="1">
-        <v>396</v>
+        <v>456</v>
       </c>
       <c r="AU1" t="s" s="1">
-        <v>419</v>
+        <v>479</v>
       </c>
       <c r="AV1" t="s" s="1">
-        <v>424</v>
+        <v>484</v>
       </c>
       <c r="AW1" t="s" s="1">
-        <v>425</v>
+        <v>485</v>
       </c>
       <c r="AX1" t="s" s="1">
-        <v>426</v>
+        <v>486</v>
       </c>
       <c r="AY1" t="s" s="1">
-        <v>437</v>
+        <v>503</v>
       </c>
       <c r="AZ1" t="s" s="1">
-        <v>438</v>
+        <v>504</v>
       </c>
     </row>
     <row r="2">
@@ -2099,7 +2297,7 @@
         <v>64</v>
       </c>
       <c r="AZ2" t="s" s="53">
-        <v>439</v>
+        <v>505</v>
       </c>
     </row>
   </sheetData>
@@ -2114,10 +2312,10 @@
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$20</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$21</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$49</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$50</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -2202,10 +2400,10 @@
       <formula2>2147483647</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="AJ2:AJ1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'library_preparation_kit'!$A$1:$A$10</formula1>
+      <formula1>'library_preparation_kit'!$A$1:$A$22</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AK2:AK1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'sample_indexing_kit'!$A$1:$A$4</formula1>
+      <formula1>'sample_indexing_kit'!$A$1:$A$15</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AM2:AM1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_technical_replicate'!$A$1:$A$2</formula1>
@@ -2215,7 +2413,7 @@
       <formula2>2147483647</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="AO2:AO1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'sequencing_reagent_kit'!$A$1:$A$16</formula1>
+      <formula1>'sequencing_reagent_kit'!$A$1:$A$21</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AS2:AS1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'preparation_instrument_vendor'!$A$1:$A$7</formula1>
@@ -2234,7 +2432,7 @@
       <formula1>'probe_hybridization_time_unit'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AX2:AX1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'oligo_probe_panel'!$A$1:$A$6</formula1>
+      <formula1>'oligo_probe_panel'!$A$1:$A$9</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AY2:AY1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_custom_probes_used'!$A$1:$A$2</formula1>
@@ -2256,26 +2454,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>266</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>267</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -2293,32 +2491,32 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>275</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -2336,22 +2534,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>257</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -2369,26 +2567,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>266</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>267</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -2406,27 +2604,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>281</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>282</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -2444,42 +2642,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>285</v>
+        <v>289</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>287</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>289</v>
+        <v>293</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>291</v>
+        <v>295</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>293</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -2497,18 +2695,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>298</v>
+        <v>302</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>300</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -2526,18 +2724,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>298</v>
+        <v>302</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>306</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -2555,18 +2753,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>298</v>
+        <v>302</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>306</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -2584,18 +2782,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>312</v>
+        <v>316</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>314</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -2898,18 +3096,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>317</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>319</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -2919,7 +3117,7 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2927,82 +3125,178 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>324</v>
+        <v>328</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>326</v>
+        <v>330</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>328</v>
+        <v>332</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>330</v>
+        <v>334</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>332</v>
+        <v>336</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>334</v>
+        <v>338</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>336</v>
+        <v>340</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>338</v>
+        <v>342</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>340</v>
+        <v>344</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>342</v>
+        <v>346</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>347</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>349</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>351</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>353</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>355</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>357</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>359</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>361</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>363</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>365</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>367</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>369</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>370</v>
       </c>
     </row>
   </sheetData>
@@ -3012,7 +3306,7 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3020,34 +3314,122 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>344</v>
+        <v>372</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>345</v>
+        <v>373</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>267</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>346</v>
+        <v>374</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>347</v>
+        <v>375</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>348</v>
+        <v>376</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>349</v>
+        <v>377</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>378</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>380</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>382</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>384</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>386</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>388</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>390</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>392</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>394</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>396</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>398</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>399</v>
       </c>
     </row>
   </sheetData>
@@ -3080,7 +3462,7 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3088,130 +3470,170 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>354</v>
+        <v>404</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>355</v>
+        <v>405</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>356</v>
+        <v>406</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>357</v>
+        <v>407</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>358</v>
+        <v>408</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>359</v>
+        <v>409</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>360</v>
+        <v>410</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>361</v>
+        <v>411</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>362</v>
+        <v>412</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>363</v>
+        <v>413</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>364</v>
+        <v>414</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>365</v>
+        <v>415</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>366</v>
+        <v>416</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>367</v>
+        <v>417</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>368</v>
+        <v>418</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>369</v>
+        <v>419</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>370</v>
+        <v>420</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>371</v>
+        <v>421</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>372</v>
+        <v>422</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>373</v>
+        <v>423</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>374</v>
+        <v>424</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>375</v>
+        <v>425</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>376</v>
+        <v>426</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>377</v>
+        <v>427</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>378</v>
+        <v>428</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>379</v>
+        <v>429</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>380</v>
+        <v>430</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>381</v>
+        <v>431</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>382</v>
+        <v>432</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>383</v>
+        <v>433</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>384</v>
+        <v>434</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>385</v>
+        <v>435</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>436</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>438</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>440</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>442</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>444</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>445</v>
       </c>
     </row>
   </sheetData>
@@ -3237,50 +3659,50 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>267</v>
+        <v>271</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>390</v>
+        <v>450</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>391</v>
+        <v>451</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>392</v>
+        <v>452</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>393</v>
+        <v>453</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>394</v>
+        <v>454</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>395</v>
+        <v>455</v>
       </c>
     </row>
   </sheetData>
@@ -3298,122 +3720,122 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>267</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>397</v>
+        <v>457</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>398</v>
+        <v>458</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>399</v>
+        <v>459</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>400</v>
+        <v>460</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>231</v>
+        <v>235</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>401</v>
+        <v>461</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>402</v>
+        <v>462</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>403</v>
+        <v>463</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>404</v>
+        <v>464</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>405</v>
+        <v>465</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>406</v>
+        <v>466</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>407</v>
+        <v>467</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>408</v>
+        <v>468</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>409</v>
+        <v>469</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>410</v>
+        <v>470</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>411</v>
+        <v>471</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>412</v>
+        <v>472</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>413</v>
+        <v>473</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>414</v>
+        <v>474</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>415</v>
+        <v>475</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>416</v>
+        <v>476</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>417</v>
+        <v>477</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>418</v>
+        <v>478</v>
       </c>
     </row>
   </sheetData>
@@ -3431,34 +3853,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>329</v>
+        <v>337</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>330</v>
+        <v>338</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>323</v>
+        <v>355</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>324</v>
+        <v>356</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>420</v>
+        <v>480</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>421</v>
+        <v>481</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>422</v>
+        <v>482</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>423</v>
+        <v>483</v>
       </c>
     </row>
   </sheetData>
@@ -3476,18 +3898,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -3497,7 +3919,7 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3505,50 +3927,74 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>427</v>
+        <v>487</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>428</v>
+        <v>488</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>429</v>
+        <v>489</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>430</v>
+        <v>490</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>337</v>
+        <v>491</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>338</v>
+        <v>492</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>431</v>
+        <v>493</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>432</v>
+        <v>494</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>433</v>
+        <v>495</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>434</v>
+        <v>496</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>435</v>
+        <v>347</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>436</v>
+        <v>348</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>497</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>499</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>501</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>502</v>
       </c>
     </row>
   </sheetData>
@@ -3704,16 +4150,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>440</v>
+        <v>506</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>441</v>
+        <v>507</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>443</v>
+        <v>509</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>445</v>
+        <v>511</v>
       </c>
     </row>
     <row r="2">
@@ -3721,13 +4167,13 @@
         <v>64</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>442</v>
+        <v>508</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>444</v>
+        <v>510</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>446</v>
+        <v>512</v>
       </c>
     </row>
   </sheetData>
@@ -3760,7 +4206,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3926,6 +4372,14 @@
         <v>140</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>141</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>142</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -3933,7 +4387,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3941,394 +4395,402 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>239</v>
+        <v>241</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>242</v>
+      </c>
+      <c r="B50" t="s" s="0">
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -4346,42 +4808,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -4399,26 +4861,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -4436,37 +4898,37 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>257</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>258</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>260</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>262</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a new library preparation kit and oligo probe kit
Closes #29
</commit_message>
<xml_diff>
--- a/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
+++ b/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
@@ -416,7 +416,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="547">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -1483,6 +1483,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000374</t>
   </si>
   <si>
+    <t>New England BioLabs; NEBNext Ultra II RNA Library Prep Kit for Illumina; PN E7770</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000377</t>
+  </si>
+  <si>
     <t>10X Genomics; Chromium Next GEM Automated Single Cell 5' Kit v2, 24 rxns; PN 1000290</t>
   </si>
   <si>
@@ -1525,6 +1531,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000260</t>
   </si>
   <si>
+    <t>10X Genomics; Chromium Next GEM Single Cell Fixed RNA Hybridization &amp; Library Kit, 4 rxns; PN 1000415</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000375</t>
+  </si>
+  <si>
     <t>Custom</t>
   </si>
   <si>
@@ -1912,6 +1924,12 @@
     <t>preparation_instrument_kit</t>
   </si>
   <si>
+    <t>10X Genomics; Chromium Next GEM Chip G Single Cell Kit, 16 rxns; PN 1000127</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000379</t>
+  </si>
+  <si>
     <t>10X Genomics; Chromium Next GEM Chip K Automated Single Cell Kit, 48 rxns; PN 1000289</t>
   </si>
   <si>
@@ -1924,6 +1942,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000367</t>
   </si>
   <si>
+    <t>10X Genomics; Chromium Next GEM Chip G Single Cell Kit, 48 rxns; PN 1000120</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000378</t>
+  </si>
+  <si>
     <t>10X Genomics; Visium FFPE Reagent Kit v2-Small, PN 1000436</t>
   </si>
   <si>
@@ -1963,6 +1987,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000364</t>
   </si>
   <si>
+    <t>10X Genomics; Chromium Next GEM Single Cell Fixed RNA Human Transcriptome Probe Kit, 64 rxns; PN 1000456</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000376</t>
+  </si>
+  <si>
     <t>10x Genomics; Visium Human Transcriptome Probe Kit-Small; PN 1000363</t>
   </si>
   <si>
@@ -2020,7 +2050,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-04-01T14:49:54-07:00</t>
+    <t>2024-04-05T13:06:47-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -2316,52 +2346,52 @@
         <v>330</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="AO1" t="s" s="1">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="AP1" t="s" s="1">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="AQ1" t="s" s="1">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="AR1" t="s" s="1">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="AS1" t="s" s="1">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="AT1" t="s" s="1">
-        <v>470</v>
+        <v>474</v>
       </c>
       <c r="AU1" t="s" s="1">
-        <v>497</v>
+        <v>501</v>
       </c>
       <c r="AV1" t="s" s="1">
-        <v>508</v>
+        <v>516</v>
       </c>
       <c r="AW1" t="s" s="1">
-        <v>509</v>
+        <v>517</v>
       </c>
       <c r="AX1" t="s" s="1">
-        <v>510</v>
+        <v>518</v>
       </c>
       <c r="AY1" t="s" s="1">
-        <v>527</v>
+        <v>537</v>
       </c>
       <c r="AZ1" t="s" s="1">
-        <v>528</v>
+        <v>538</v>
       </c>
     </row>
     <row r="2">
@@ -2369,7 +2399,7 @@
         <v>64</v>
       </c>
       <c r="AZ2" t="s" s="53">
-        <v>529</v>
+        <v>539</v>
       </c>
     </row>
   </sheetData>
@@ -2472,7 +2502,7 @@
       <formula2>2147483647</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="AJ2:AJ1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'library_preparation_kit'!$A$1:$A$25</formula1>
+      <formula1>'library_preparation_kit'!$A$1:$A$27</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AK2:AK1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'sample_indexing_kit'!$A$1:$A$15</formula1>
@@ -2494,7 +2524,7 @@
       <formula1>'preparation_instrument_model'!$A$1:$A$18</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AU2:AU1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_instrument_kit'!$A$1:$A$7</formula1>
+      <formula1>'preparation_instrument_kit'!$A$1:$A$9</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="between" sqref="AV2:AV1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be a number" showErrorMessage="true">
       <formula1>-3.4028235E38</formula1>
@@ -2504,7 +2534,7 @@
       <formula1>'probe_hybridization_time_unit'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AX2:AX1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'oligo_probe_panel'!$A$1:$A$9</formula1>
+      <formula1>'oligo_probe_panel'!$A$1:$A$10</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AY2:AY1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_custom_probes_used'!$A$1:$A$2</formula1>
@@ -3189,7 +3219,7 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3393,6 +3423,22 @@
       </c>
       <c r="B25" t="s" s="0">
         <v>380</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>381</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>383</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>384</v>
       </c>
     </row>
   </sheetData>
@@ -3410,10 +3456,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>383</v>
+        <v>387</v>
       </c>
     </row>
     <row r="2">
@@ -3426,106 +3472,106 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>385</v>
+        <v>389</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>387</v>
+        <v>391</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>391</v>
+        <v>395</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>395</v>
+        <v>399</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>397</v>
+        <v>401</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>399</v>
+        <v>403</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>401</v>
+        <v>405</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>403</v>
+        <v>407</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>405</v>
+        <v>409</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>407</v>
+        <v>411</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>409</v>
+        <v>413</v>
       </c>
     </row>
   </sheetData>
@@ -3566,178 +3612,178 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>415</v>
+        <v>419</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>417</v>
+        <v>421</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>419</v>
+        <v>423</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>421</v>
+        <v>425</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>425</v>
+        <v>429</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>427</v>
+        <v>431</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>429</v>
+        <v>433</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>431</v>
+        <v>435</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>433</v>
+        <v>437</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>435</v>
+        <v>439</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>437</v>
+        <v>441</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>439</v>
+        <v>443</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>441</v>
+        <v>445</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>443</v>
+        <v>447</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>445</v>
+        <v>449</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>447</v>
+        <v>451</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>449</v>
+        <v>453</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>451</v>
+        <v>455</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>453</v>
+        <v>457</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>455</v>
+        <v>459</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>457</v>
+        <v>461</v>
       </c>
     </row>
   </sheetData>
@@ -3787,26 +3833,26 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>463</v>
+        <v>467</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>465</v>
+        <v>469</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>467</v>
+        <v>471</v>
       </c>
     </row>
     <row r="8">
@@ -3819,10 +3865,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>468</v>
+        <v>472</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>469</v>
+        <v>473</v>
       </c>
     </row>
   </sheetData>
@@ -3856,10 +3902,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>472</v>
+        <v>476</v>
       </c>
     </row>
     <row r="4">
@@ -3872,10 +3918,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>474</v>
+        <v>478</v>
       </c>
     </row>
     <row r="6">
@@ -3896,90 +3942,90 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>475</v>
+        <v>479</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>476</v>
+        <v>480</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>478</v>
+        <v>482</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>480</v>
+        <v>484</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>482</v>
+        <v>486</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>484</v>
+        <v>488</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>486</v>
+        <v>490</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>488</v>
+        <v>492</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>490</v>
+        <v>494</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>491</v>
+        <v>495</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>492</v>
+        <v>496</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>493</v>
+        <v>497</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>494</v>
+        <v>498</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>495</v>
+        <v>499</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>496</v>
+        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -3989,7 +4035,7 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3997,58 +4043,74 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>498</v>
+        <v>502</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>499</v>
+        <v>503</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>375</v>
+        <v>504</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>376</v>
+        <v>505</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>365</v>
+        <v>379</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>366</v>
+        <v>380</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>500</v>
+        <v>367</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>501</v>
+        <v>368</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>502</v>
+        <v>506</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>503</v>
+        <v>507</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>505</v>
+        <v>509</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>506</v>
+        <v>510</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>507</v>
+        <v>511</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>512</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>514</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>515</v>
       </c>
     </row>
   </sheetData>
@@ -4087,7 +4149,7 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4095,74 +4157,82 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>511</v>
+        <v>519</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>512</v>
+        <v>520</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>513</v>
+        <v>521</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>514</v>
+        <v>522</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>515</v>
+        <v>523</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>516</v>
+        <v>524</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>517</v>
+        <v>525</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>518</v>
+        <v>526</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>519</v>
+        <v>527</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>520</v>
+        <v>528</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>369</v>
+        <v>529</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>370</v>
+        <v>530</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>521</v>
+        <v>373</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>522</v>
+        <v>374</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>523</v>
+        <v>531</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>524</v>
+        <v>532</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>525</v>
+        <v>533</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>526</v>
+        <v>534</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>535</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>536</v>
       </c>
     </row>
   </sheetData>
@@ -4318,16 +4388,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>530</v>
+        <v>540</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>531</v>
+        <v>541</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>533</v>
+        <v>543</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>535</v>
+        <v>545</v>
       </c>
     </row>
     <row r="2">
@@ -4335,13 +4405,13 @@
         <v>64</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>532</v>
+        <v>542</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>534</v>
+        <v>544</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>536</v>
+        <v>546</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new UMI size, offset and barcode size
Closes #36
Closes #37
Closes #38
</commit_message>
<xml_diff>
--- a/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
+++ b/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
@@ -416,7 +416,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="553">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -1261,6 +1261,9 @@
     <t>14</t>
   </si>
   <si>
+    <t>8,8</t>
+  </si>
+  <si>
     <t>16</t>
   </si>
   <si>
@@ -1273,6 +1276,9 @@
     <t>umi_offset</t>
   </si>
   <si>
+    <t>34</t>
+  </si>
+  <si>
     <t>36</t>
   </si>
   <si>
@@ -1594,6 +1600,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000348</t>
   </si>
   <si>
+    <t>10X Genomics; Chromium i7 Sample Index Plate (96 rxn); PN 220103</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000380</t>
+  </si>
+  <si>
     <t>NanoString Technologies; GeoMx Seq Code Pack; PN GMX-NGS-SEQ-AB</t>
   </si>
   <si>
@@ -1780,6 +1792,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000287</t>
   </si>
   <si>
+    <t>Illumina; NextSeq 500/550 Hi Output Kit 75 Cycles v2.5; PN 20024906</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000381</t>
+  </si>
+  <si>
     <t>Illumina; NovaSeq 6000 S4 Reagent Kit v1.5 (300 cycles); PN 20028312</t>
   </si>
   <si>
@@ -2050,7 +2068,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-04-17T14:18:53-07:00</t>
+    <t>2024-04-23T15:02:39-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -2289,109 +2307,109 @@
         <v>278</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="AO1" t="s" s="1">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="AP1" t="s" s="1">
-        <v>462</v>
+        <v>468</v>
       </c>
       <c r="AQ1" t="s" s="1">
-        <v>463</v>
+        <v>469</v>
       </c>
       <c r="AR1" t="s" s="1">
-        <v>464</v>
+        <v>470</v>
       </c>
       <c r="AS1" t="s" s="1">
-        <v>465</v>
+        <v>471</v>
       </c>
       <c r="AT1" t="s" s="1">
-        <v>474</v>
+        <v>480</v>
       </c>
       <c r="AU1" t="s" s="1">
-        <v>501</v>
+        <v>507</v>
       </c>
       <c r="AV1" t="s" s="1">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="AW1" t="s" s="1">
-        <v>517</v>
+        <v>523</v>
       </c>
       <c r="AX1" t="s" s="1">
-        <v>518</v>
+        <v>524</v>
       </c>
       <c r="AY1" t="s" s="1">
-        <v>537</v>
+        <v>543</v>
       </c>
       <c r="AZ1" t="s" s="1">
-        <v>538</v>
+        <v>544</v>
       </c>
     </row>
     <row r="2">
@@ -2399,7 +2417,7 @@
         <v>64</v>
       </c>
       <c r="AZ2" t="s" s="53">
-        <v>539</v>
+        <v>545</v>
       </c>
     </row>
   </sheetData>
@@ -2440,16 +2458,16 @@
       <formula1>'barcode_read'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="Q2:Q1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'barcode_size'!$A$1:$A$6</formula1>
+      <formula1>'barcode_size'!$A$1:$A$7</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="R2:R1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'umi_offset'!$A$1:$A$4</formula1>
+      <formula1>'umi_offset'!$A$1:$A$5</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="S2:S1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'umi_read'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="T2:T1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'umi_size'!$A$1:$A$5</formula1>
+      <formula1>'umi_size'!$A$1:$A$6</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="U2:U1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'assay_input_entity'!$A$1:$A$5</formula1>
@@ -2505,7 +2523,7 @@
       <formula1>'library_preparation_kit'!$A$1:$A$27</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AK2:AK1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'sample_indexing_kit'!$A$1:$A$15</formula1>
+      <formula1>'sample_indexing_kit'!$A$1:$A$16</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AM2:AM1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_technical_replicate'!$A$1:$A$2</formula1>
@@ -2515,7 +2533,7 @@
       <formula2>2147483647</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="AO2:AO1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'sequencing_reagent_kit'!$A$1:$A$22</formula1>
+      <formula1>'sequencing_reagent_kit'!$A$1:$A$23</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AS2:AS1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'preparation_instrument_vendor'!$A$1:$A$9</formula1>
@@ -2585,7 +2603,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2621,6 +2639,11 @@
         <v>283</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>284</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -2628,7 +2651,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2641,17 +2664,22 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>267</v>
+        <v>287</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>281</v>
+        <v>267</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -2698,7 +2726,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2706,27 +2734,32 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>267</v>
+        <v>280</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>289</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>290</v>
+        <v>291</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -2744,42 +2777,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -2797,18 +2830,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -2826,18 +2859,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>
@@ -2855,18 +2888,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>
@@ -2884,18 +2917,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -3198,18 +3231,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -3227,218 +3260,218 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>334</v>
+        <v>336</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>370</v>
+        <v>372</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>374</v>
+        <v>376</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>376</v>
+        <v>378</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>378</v>
+        <v>380</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>380</v>
+        <v>382</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>382</v>
+        <v>384</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>384</v>
+        <v>386</v>
       </c>
     </row>
   </sheetData>
@@ -3448,7 +3481,7 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3456,10 +3489,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>387</v>
+        <v>389</v>
       </c>
     </row>
     <row r="2">
@@ -3472,106 +3505,114 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>389</v>
+        <v>391</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>391</v>
+        <v>393</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>393</v>
+        <v>395</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>395</v>
+        <v>397</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>397</v>
+        <v>399</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>401</v>
+        <v>403</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>403</v>
+        <v>405</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>405</v>
+        <v>407</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>407</v>
+        <v>409</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>409</v>
+        <v>411</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>413</v>
+        <v>415</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>416</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -3604,7 +3645,7 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3612,178 +3653,186 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>419</v>
+        <v>423</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>421</v>
+        <v>425</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>425</v>
+        <v>429</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>427</v>
+        <v>431</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>429</v>
+        <v>433</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>431</v>
+        <v>435</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>433</v>
+        <v>437</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>435</v>
+        <v>439</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>437</v>
+        <v>441</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>439</v>
+        <v>443</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>441</v>
+        <v>445</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>443</v>
+        <v>447</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>445</v>
+        <v>449</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>447</v>
+        <v>451</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>449</v>
+        <v>453</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>451</v>
+        <v>455</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>453</v>
+        <v>457</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>455</v>
+        <v>459</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>457</v>
+        <v>461</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>459</v>
+        <v>463</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>461</v>
+        <v>465</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>466</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>467</v>
       </c>
     </row>
   </sheetData>
@@ -3833,26 +3882,26 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>466</v>
+        <v>472</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>467</v>
+        <v>473</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>469</v>
+        <v>475</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>470</v>
+        <v>476</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>471</v>
+        <v>477</v>
       </c>
     </row>
     <row r="8">
@@ -3865,10 +3914,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>472</v>
+        <v>478</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>473</v>
+        <v>479</v>
       </c>
     </row>
   </sheetData>
@@ -3902,10 +3951,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>475</v>
+        <v>481</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>476</v>
+        <v>482</v>
       </c>
     </row>
     <row r="4">
@@ -3918,10 +3967,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>477</v>
+        <v>483</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>478</v>
+        <v>484</v>
       </c>
     </row>
     <row r="6">
@@ -3942,90 +3991,90 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>479</v>
+        <v>485</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>480</v>
+        <v>486</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>481</v>
+        <v>487</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>482</v>
+        <v>488</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>483</v>
+        <v>489</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>484</v>
+        <v>490</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>485</v>
+        <v>491</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>486</v>
+        <v>492</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>487</v>
+        <v>493</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>488</v>
+        <v>494</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>489</v>
+        <v>495</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>490</v>
+        <v>496</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>491</v>
+        <v>497</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>492</v>
+        <v>498</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>493</v>
+        <v>499</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>494</v>
+        <v>500</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>495</v>
+        <v>501</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>496</v>
+        <v>502</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>497</v>
+        <v>503</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>498</v>
+        <v>504</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>500</v>
+        <v>506</v>
       </c>
     </row>
   </sheetData>
@@ -4043,74 +4092,74 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>502</v>
+        <v>508</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>503</v>
+        <v>509</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>504</v>
+        <v>510</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>505</v>
+        <v>511</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>380</v>
+        <v>382</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>506</v>
+        <v>512</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>507</v>
+        <v>513</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>508</v>
+        <v>514</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>509</v>
+        <v>515</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>510</v>
+        <v>516</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>511</v>
+        <v>517</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>512</v>
+        <v>518</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>513</v>
+        <v>519</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>514</v>
+        <v>520</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>515</v>
+        <v>521</v>
       </c>
     </row>
   </sheetData>
@@ -4157,82 +4206,82 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>519</v>
+        <v>525</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>520</v>
+        <v>526</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>521</v>
+        <v>527</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>522</v>
+        <v>528</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>523</v>
+        <v>529</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>524</v>
+        <v>530</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>525</v>
+        <v>531</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>526</v>
+        <v>532</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>528</v>
+        <v>534</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>529</v>
+        <v>535</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>530</v>
+        <v>536</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>374</v>
+        <v>376</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>531</v>
+        <v>537</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>532</v>
+        <v>538</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>533</v>
+        <v>539</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>534</v>
+        <v>540</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>535</v>
+        <v>541</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>536</v>
+        <v>542</v>
       </c>
     </row>
   </sheetData>
@@ -4388,16 +4437,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>540</v>
+        <v>546</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>541</v>
+        <v>547</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>543</v>
+        <v>549</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>545</v>
+        <v>551</v>
       </c>
     </row>
     <row r="2">
@@ -4405,13 +4454,13 @@
         <v>64</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>542</v>
+        <v>548</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>544</v>
+        <v>550</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>546</v>
+        <v>552</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replaced some oligo probe panels
Closes #39
</commit_message>
<xml_diff>
--- a/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
+++ b/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
@@ -1993,12 +1993,6 @@
     <t>oligo_probe_panel</t>
   </si>
   <si>
-    <t>10x Genomics; Chromium Fixed RNA Kit, Human Transcriptome 4 rxns x 16 BC; PN 1000476</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000308</t>
-  </si>
-  <si>
     <t>NanoString Technologies; GeoMx Mouse Whole Transcriptome Atlas, 4 slides; PN GMX-RNA-NGS-MsWTA-4</t>
   </si>
   <si>
@@ -2011,6 +2005,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000376</t>
   </si>
   <si>
+    <t>10x Genomics; Visium Human Transcriptome Probe Kit-Large; PN 1000364</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000383</t>
+  </si>
+  <si>
     <t>10x Genomics; Visium Human Transcriptome Probe Kit-Small; PN 1000363</t>
   </si>
   <si>
@@ -2035,18 +2035,18 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000363</t>
   </si>
   <si>
-    <t>10x Genomics; Chromium Fixed RNA Kit, Human Transcriptome 4 rxns x 4 BC; PN 1000475</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000307</t>
-  </si>
-  <si>
     <t>10x Genomics; Visium Human Transcriptome Probe Kit v2 - Small; PN 1000466</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000274</t>
   </si>
   <si>
+    <t>10X Genomics; Chromium Next GEM Single Cell Fixed RNA Human Transcriptome Probe Kit, 16 rxns; PN 1000420</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000382</t>
+  </si>
+  <si>
     <t>is_custom_probes_used</t>
   </si>
   <si>
@@ -2068,7 +2068,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-04-23T15:02:39-07:00</t>
+    <t>2024-05-09T09:47:42-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>

</xml_diff>

<commit_message>
Adding a new oligo probe panel
Closes #58
</commit_message>
<xml_diff>
--- a/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
+++ b/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
@@ -416,7 +416,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="569">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -841,6 +841,12 @@
     <t>https://identifiers.org/RRID:SCR_023603</t>
   </si>
   <si>
+    <t>10x Genomics</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023672</t>
+  </si>
+  <si>
     <t>NanoString</t>
   </si>
   <si>
@@ -1882,12 +1888,6 @@
     <t>https://identifiers.org/RRID:SCR_023734</t>
   </si>
   <si>
-    <t>10x Genomics</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023672</t>
-  </si>
-  <si>
     <t>SunChrom</t>
   </si>
   <si>
@@ -2035,6 +2035,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000364</t>
   </si>
   <si>
+    <t>10x Genomics; Chromium Next GEM Single Cell Fixed RNA Mouse Transcriptome Probe Kit, 64 rxns; PN 1000492</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000393</t>
+  </si>
+  <si>
     <t>10X Genomics; Chromium Next GEM Single Cell Fixed RNA Human Transcriptome Probe Kit, 64 rxns; PN 1000456</t>
   </si>
   <si>
@@ -2110,7 +2116,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-11-01T11:48:43-07:00</t>
+    <t>2024-11-18T14:20:48-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -2319,118 +2325,118 @@
         <v>110</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="AO1" t="s" s="1">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="AP1" t="s" s="1">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="AQ1" t="s" s="1">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="AR1" t="s" s="1">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="AS1" t="s" s="1">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="AT1" t="s" s="1">
         <v>492</v>
@@ -2448,10 +2454,10 @@
         <v>536</v>
       </c>
       <c r="AY1" t="s" s="1">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="AZ1" t="s" s="1">
-        <v>558</v>
+        <v>560</v>
       </c>
     </row>
     <row r="2">
@@ -2459,7 +2465,7 @@
         <v>68</v>
       </c>
       <c r="AZ2" t="s" s="53">
-        <v>559</v>
+        <v>561</v>
       </c>
     </row>
   </sheetData>
@@ -2474,7 +2480,7 @@
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$22</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$23</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'acquisition_instrument_model'!$A$1:$A$52</formula1>
@@ -2594,7 +2600,7 @@
       <formula1>'probe_hybridization_time_unit'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AX2:AX1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'oligo_probe_panel'!$A$1:$A$11</formula1>
+      <formula1>'oligo_probe_panel'!$A$1:$A$12</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AY2:AY1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_custom_probes_used'!$A$1:$A$2</formula1>
@@ -2616,26 +2622,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -2653,37 +2659,37 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2701,27 +2707,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2739,26 +2745,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -2776,32 +2782,32 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2819,42 +2825,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -2872,18 +2878,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -2901,18 +2907,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -2930,18 +2936,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -2959,18 +2965,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>334</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -3289,18 +3295,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>339</v>
+        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -3318,218 +3324,218 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>370</v>
+        <v>372</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>374</v>
+        <v>376</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>376</v>
+        <v>378</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>378</v>
+        <v>380</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>380</v>
+        <v>382</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>382</v>
+        <v>384</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>384</v>
+        <v>386</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>386</v>
+        <v>388</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>388</v>
+        <v>390</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>392</v>
+        <v>394</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
   </sheetData>
@@ -3547,138 +3553,138 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>401</v>
+        <v>403</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>403</v>
+        <v>405</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>405</v>
+        <v>407</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>407</v>
+        <v>409</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>409</v>
+        <v>411</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>413</v>
+        <v>415</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>386</v>
+        <v>388</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>415</v>
+        <v>417</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>417</v>
+        <v>419</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>419</v>
+        <v>421</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>421</v>
+        <v>423</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>423</v>
+        <v>425</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>425</v>
+        <v>427</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
   </sheetData>
@@ -3719,202 +3725,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>433</v>
+        <v>435</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>435</v>
+        <v>437</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>437</v>
+        <v>439</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>439</v>
+        <v>441</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>441</v>
+        <v>443</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>443</v>
+        <v>445</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>445</v>
+        <v>447</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>447</v>
+        <v>449</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>449</v>
+        <v>451</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>451</v>
+        <v>453</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>453</v>
+        <v>455</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>455</v>
+        <v>457</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>459</v>
+        <v>461</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>386</v>
+        <v>388</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>461</v>
+        <v>463</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>463</v>
+        <v>465</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>465</v>
+        <v>467</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>467</v>
+        <v>469</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>469</v>
+        <v>471</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>471</v>
+        <v>473</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>473</v>
+        <v>475</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>475</v>
+        <v>477</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>477</v>
+        <v>479</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>479</v>
+        <v>481</v>
       </c>
     </row>
   </sheetData>
@@ -3948,10 +3954,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4">
@@ -3964,34 +3970,34 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>485</v>
+        <v>487</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>487</v>
+        <v>489</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>488</v>
+        <v>141</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>489</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9">
@@ -4017,18 +4023,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3">
@@ -4041,10 +4047,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5">
@@ -4057,18 +4063,18 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8">
@@ -4190,18 +4196,18 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>392</v>
+        <v>394</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>380</v>
+        <v>382</v>
       </c>
     </row>
     <row r="5">
@@ -4230,10 +4236,10 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>386</v>
+        <v>388</v>
       </c>
     </row>
     <row r="9">
@@ -4267,18 +4273,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -4288,7 +4294,7 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4344,18 +4350,18 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>385</v>
+        <v>549</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>386</v>
+        <v>550</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>549</v>
+        <v>387</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>550</v>
+        <v>388</v>
       </c>
     </row>
     <row r="9">
@@ -4380,6 +4386,14 @@
       </c>
       <c r="B11" t="s" s="0">
         <v>556</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>557</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>558</v>
       </c>
     </row>
   </sheetData>
@@ -4559,16 +4573,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>565</v>
+        <v>567</v>
       </c>
     </row>
     <row r="2">
@@ -4576,13 +4590,13 @@
         <v>68</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>566</v>
+        <v>568</v>
       </c>
     </row>
   </sheetData>
@@ -4615,7 +4629,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4795,6 +4809,14 @@
       </c>
       <c r="B22" t="s" s="0">
         <v>154</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>155</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -4812,418 +4834,418 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -5241,42 +5263,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -5294,26 +5316,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -5331,37 +5353,37 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a new library preparation kit
Closes #59
</commit_message>
<xml_diff>
--- a/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
+++ b/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
@@ -416,7 +416,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="571">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -1543,6 +1543,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000265</t>
   </si>
   <si>
+    <t>10x Genomics; Chromium GEM-X Single Cell 5' Kit v3, 16 rxns; PN 1000699</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000394</t>
+  </si>
+  <si>
     <t>Parse Biosciences; Evercode WT Mini v2 Kit, 12 rxns; PN ECW02010</t>
   </si>
   <si>
@@ -1567,24 +1573,24 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000251</t>
   </si>
   <si>
-    <t>10X Genomics; Chromium Single Cell 3' GEM, Library &amp; Gel Bead Kit v3, 4 rxns PN 1000092</t>
+    <t>10X Genomics; Chromium Next GEM Single Cell Fixed RNA Hybridization &amp; Library Kit, 4 rxns; PN 1000415</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000375</t>
+  </si>
+  <si>
+    <t>Custom</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C65167</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium Single Cell 3' GEM, Library &amp; Gel Bead Kit v3, 4 rxns; PN 1000092</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000260</t>
   </si>
   <si>
-    <t>10X Genomics; Chromium Next GEM Single Cell Fixed RNA Hybridization &amp; Library Kit, 4 rxns; PN 1000415</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000375</t>
-  </si>
-  <si>
-    <t>Custom</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C65167</t>
-  </si>
-  <si>
     <t>10X Genomics; Chromium Single Cell 3' Library &amp; Gel Bead Kit, 4 rxns; PN 120267</t>
   </si>
   <si>
@@ -2116,7 +2122,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-11-18T14:20:48-08:00</t>
+    <t>2024-12-03T17:20:00-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -2412,52 +2418,52 @@
         <v>344</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="AO1" t="s" s="1">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="AP1" t="s" s="1">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="AQ1" t="s" s="1">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="AR1" t="s" s="1">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="AS1" t="s" s="1">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="AT1" t="s" s="1">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="AU1" t="s" s="1">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="AV1" t="s" s="1">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="AW1" t="s" s="1">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="AX1" t="s" s="1">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="AY1" t="s" s="1">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="AZ1" t="s" s="1">
-        <v>560</v>
+        <v>562</v>
       </c>
     </row>
     <row r="2">
@@ -2465,7 +2471,7 @@
         <v>68</v>
       </c>
       <c r="AZ2" t="s" s="53">
-        <v>561</v>
+        <v>563</v>
       </c>
     </row>
   </sheetData>
@@ -2568,7 +2574,7 @@
       <formula2>2147483647</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="AJ2:AJ1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'library_preparation_kit'!$A$1:$A$27</formula1>
+      <formula1>'library_preparation_kit'!$A$1:$A$28</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AK2:AK1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'sample_indexing_kit'!$A$1:$A$17</formula1>
@@ -3316,7 +3322,7 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3536,6 +3542,14 @@
       </c>
       <c r="B27" t="s" s="0">
         <v>398</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>399</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>400</v>
       </c>
     </row>
   </sheetData>
@@ -3553,10 +3567,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>401</v>
+        <v>403</v>
       </c>
     </row>
     <row r="2">
@@ -3569,58 +3583,58 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>403</v>
+        <v>405</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>405</v>
+        <v>407</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>407</v>
+        <v>409</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>409</v>
+        <v>411</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>413</v>
+        <v>415</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>415</v>
+        <v>417</v>
       </c>
     </row>
     <row r="10">
@@ -3633,58 +3647,58 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>417</v>
+        <v>419</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>419</v>
+        <v>421</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>421</v>
+        <v>423</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>423</v>
+        <v>425</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>425</v>
+        <v>427</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>429</v>
+        <v>431</v>
       </c>
     </row>
   </sheetData>
@@ -3725,114 +3739,114 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>435</v>
+        <v>437</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>437</v>
+        <v>439</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>439</v>
+        <v>441</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>441</v>
+        <v>443</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>443</v>
+        <v>445</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>445</v>
+        <v>447</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>447</v>
+        <v>449</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>449</v>
+        <v>451</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>451</v>
+        <v>453</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>453</v>
+        <v>455</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>455</v>
+        <v>457</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>459</v>
+        <v>461</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>461</v>
+        <v>463</v>
       </c>
     </row>
     <row r="15">
@@ -3845,82 +3859,82 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>463</v>
+        <v>465</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>465</v>
+        <v>467</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>467</v>
+        <v>469</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>469</v>
+        <v>471</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>471</v>
+        <v>473</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>473</v>
+        <v>475</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>475</v>
+        <v>477</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>477</v>
+        <v>479</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>479</v>
+        <v>481</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>481</v>
+        <v>483</v>
       </c>
     </row>
   </sheetData>
@@ -3970,18 +3984,18 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>487</v>
+        <v>489</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="7">
@@ -4002,10 +4016,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>491</v>
+        <v>493</v>
       </c>
     </row>
   </sheetData>
@@ -4039,10 +4053,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>494</v>
+        <v>496</v>
       </c>
     </row>
     <row r="4">
@@ -4055,10 +4069,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>496</v>
+        <v>498</v>
       </c>
     </row>
     <row r="6">
@@ -4079,90 +4093,90 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>498</v>
+        <v>500</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>500</v>
+        <v>502</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>502</v>
+        <v>504</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>504</v>
+        <v>506</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>506</v>
+        <v>508</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>508</v>
+        <v>510</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>510</v>
+        <v>512</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>512</v>
+        <v>514</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>514</v>
+        <v>516</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>516</v>
+        <v>518</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>518</v>
+        <v>520</v>
       </c>
     </row>
   </sheetData>
@@ -4180,58 +4194,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>521</v>
+        <v>523</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>523</v>
+        <v>525</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>382</v>
+        <v>384</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>525</v>
+        <v>527</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>527</v>
+        <v>529</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>529</v>
+        <v>531</v>
       </c>
     </row>
     <row r="8">
@@ -4244,18 +4258,18 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>531</v>
+        <v>533</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>533</v>
+        <v>535</v>
       </c>
     </row>
   </sheetData>
@@ -4302,58 +4316,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>544</v>
+        <v>546</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>546</v>
+        <v>548</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>548</v>
+        <v>550</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>550</v>
+        <v>552</v>
       </c>
     </row>
     <row r="8">
@@ -4366,34 +4380,34 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>552</v>
+        <v>554</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>554</v>
+        <v>556</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>556</v>
+        <v>558</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>558</v>
+        <v>560</v>
       </c>
     </row>
   </sheetData>
@@ -4573,16 +4587,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>567</v>
+        <v>569</v>
       </c>
     </row>
     <row r="2">
@@ -4590,13 +4604,13 @@
         <v>68</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>568</v>
+        <v>570</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new library preparation kits and a preparation instrument kit
Closes #61 and #62
</commit_message>
<xml_diff>
--- a/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
+++ b/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
@@ -416,7 +416,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="583">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -556,6 +556,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000201</t>
   </si>
   <si>
+    <t>seqFISH</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000397</t>
+  </si>
+  <si>
     <t>2D Imaging Mass Cytometry</t>
   </si>
   <si>
@@ -580,6 +586,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000209</t>
   </si>
   <si>
+    <t>DART-FISH</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000396</t>
+  </si>
+  <si>
     <t>Resolve</t>
   </si>
   <si>
@@ -1495,6 +1507,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000337</t>
   </si>
   <si>
+    <t>10x Genomics; Library Construction Kit C, 16 rxns; PN 1000694</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000399</t>
+  </si>
+  <si>
     <t>10X Genomics; Chromium Next GEM Single Cell 3' HT Kit v3.1, 48 rxns; PN 1000348</t>
   </si>
   <si>
@@ -1507,6 +1525,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000334</t>
   </si>
   <si>
+    <t>10x Genomics; Library Construction Kit C, 4 rxns; PN 1000689</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000398</t>
+  </si>
+  <si>
     <t>10X Genomics; Visium CytAssist Spatial Gene Expression for FFPE, Human Transcriptome, 11 mm, 2 reactions; PN 1000522</t>
   </si>
   <si>
@@ -1996,6 +2020,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000373</t>
   </si>
   <si>
+    <t>10x Genomics; Chromium GEM-X Single Cell 3' Kit v4, 16 rxns; PN 1000691</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000400</t>
+  </si>
+  <si>
     <t>10X Genomics; Chromium Next GEM Chip K Single Cell Kit, 48 rxns; PN 1000286</t>
   </si>
   <si>
@@ -2047,24 +2077,48 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000393</t>
   </si>
   <si>
+    <t>10x Genomics; Visium Human Transcriptome Probe Kit-Large; PN 1000364</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000383</t>
+  </si>
+  <si>
+    <t>10x Genomics; Visium Human Transcriptome Probe Kit-Small; PN 1000363</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000326</t>
+  </si>
+  <si>
+    <t>NanoString Technologies; GeoMx Human Whole Transcriptome Atlas, 4 slides; PN GMX-RNA-NGS-HuWTA-4</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000363</t>
+  </si>
+  <si>
+    <t>10x Genomics; Chromium Fixed RNA Kit, Human Transcriptome 4 rxns x 4 BC; PN 1000475</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000307</t>
+  </si>
+  <si>
+    <t>10x Genomics; Visium Human Transcriptome Probe Kit v2 - Small; PN 1000466</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000274</t>
+  </si>
+  <si>
+    <t>10x Genomics; Xenium Human Multi-Tissue and Cancer Panel v1; PN 1000626</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000395</t>
+  </si>
+  <si>
     <t>10X Genomics; Chromium Next GEM Single Cell Fixed RNA Human Transcriptome Probe Kit, 64 rxns; PN 1000456</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000376</t>
   </si>
   <si>
-    <t>10x Genomics; Visium Human Transcriptome Probe Kit-Large; PN 1000364</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000383</t>
-  </si>
-  <si>
-    <t>10x Genomics; Visium Human Transcriptome Probe Kit-Small; PN 1000363</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000326</t>
-  </si>
-  <si>
     <t>10x Genomics; Chromium Fixed RNA Kit, Human Transcriptome, 4 rxns x 1 BC; PN 1000474</t>
   </si>
   <si>
@@ -2077,24 +2131,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000362</t>
   </si>
   <si>
-    <t>NanoString Technologies; GeoMx Human Whole Transcriptome Atlas, 4 slides; PN GMX-RNA-NGS-HuWTA-4</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000363</t>
-  </si>
-  <si>
-    <t>10x Genomics; Chromium Fixed RNA Kit, Human Transcriptome 4 rxns x 4 BC; PN 1000475</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000307</t>
-  </si>
-  <si>
-    <t>10x Genomics; Visium Human Transcriptome Probe Kit v2 - Small; PN 1000466</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000274</t>
-  </si>
-  <si>
     <t>10X Genomics; Chromium Next GEM Single Cell Fixed RNA Human Transcriptome Probe Kit, 16 rxns; PN 1000420</t>
   </si>
   <si>
@@ -2122,7 +2158,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-12-03T17:20:00-08:00</t>
+    <t>2024-12-11T14:15:33-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -2322,162 +2358,162 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>401</v>
+        <v>409</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="AO1" t="s" s="1">
-        <v>435</v>
+        <v>443</v>
       </c>
       <c r="AP1" t="s" s="1">
-        <v>484</v>
+        <v>492</v>
       </c>
       <c r="AQ1" t="s" s="1">
-        <v>485</v>
+        <v>493</v>
       </c>
       <c r="AR1" t="s" s="1">
-        <v>486</v>
+        <v>494</v>
       </c>
       <c r="AS1" t="s" s="1">
-        <v>487</v>
+        <v>495</v>
       </c>
       <c r="AT1" t="s" s="1">
-        <v>494</v>
+        <v>502</v>
       </c>
       <c r="AU1" t="s" s="1">
-        <v>521</v>
+        <v>529</v>
       </c>
       <c r="AV1" t="s" s="1">
-        <v>536</v>
+        <v>546</v>
       </c>
       <c r="AW1" t="s" s="1">
-        <v>537</v>
+        <v>547</v>
       </c>
       <c r="AX1" t="s" s="1">
-        <v>538</v>
+        <v>548</v>
       </c>
       <c r="AY1" t="s" s="1">
-        <v>561</v>
+        <v>573</v>
       </c>
       <c r="AZ1" t="s" s="1">
-        <v>562</v>
+        <v>574</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="AZ2" t="s" s="53">
-        <v>563</v>
+        <v>575</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="41">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$36</formula1>
+      <formula1>'dataset_type'!$A$1:$A$38</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'analyte_class'!$A$1:$A$15</formula1>
@@ -2574,7 +2610,7 @@
       <formula2>2147483647</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="AJ2:AJ1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'library_preparation_kit'!$A$1:$A$28</formula1>
+      <formula1>'library_preparation_kit'!$A$1:$A$30</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AK2:AK1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'sample_indexing_kit'!$A$1:$A$17</formula1>
@@ -2596,7 +2632,7 @@
       <formula1>'preparation_instrument_model'!$A$1:$A$18</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AU2:AU1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_instrument_kit'!$A$1:$A$10</formula1>
+      <formula1>'preparation_instrument_kit'!$A$1:$A$11</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="between" sqref="AV2:AV1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be a number" showErrorMessage="true">
       <formula1>-3.4028235E38</formula1>
@@ -2606,7 +2642,7 @@
       <formula1>'probe_hybridization_time_unit'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AX2:AX1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'oligo_probe_panel'!$A$1:$A$12</formula1>
+      <formula1>'oligo_probe_panel'!$A$1:$A$13</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AY2:AY1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_custom_probes_used'!$A$1:$A$2</formula1>
@@ -2628,26 +2664,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>287</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>289</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -2665,37 +2701,37 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>291</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>292</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>293</v>
+        <v>297</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>294</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>295</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -2713,27 +2749,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>279</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>292</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>298</v>
+        <v>302</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>299</v>
+        <v>303</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -2751,26 +2787,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>287</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>289</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -2788,32 +2824,32 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>302</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>303</v>
+        <v>307</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>304</v>
+        <v>308</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>291</v>
+        <v>295</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -2831,42 +2867,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>307</v>
+        <v>311</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>309</v>
+        <v>313</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>311</v>
+        <v>315</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>313</v>
+        <v>317</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -2884,18 +2920,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>320</v>
+        <v>324</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>322</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -2913,18 +2949,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>328</v>
+        <v>332</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>322</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -2942,18 +2978,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>328</v>
+        <v>332</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>322</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -2971,18 +3007,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>334</v>
+        <v>338</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>336</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -2992,7 +3028,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3284,6 +3320,22 @@
       </c>
       <c r="B36" t="s" s="0">
         <v>75</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="B37" t="s" s="0">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="B38" t="s" s="0">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -3301,18 +3353,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>339</v>
+        <v>343</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>341</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -3322,7 +3374,7 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3330,226 +3382,242 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>346</v>
+        <v>350</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>348</v>
+        <v>352</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>350</v>
+        <v>354</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>352</v>
+        <v>356</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>354</v>
+        <v>358</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>356</v>
+        <v>360</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>358</v>
+        <v>362</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>360</v>
+        <v>364</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>362</v>
+        <v>366</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>364</v>
+        <v>368</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>366</v>
+        <v>370</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>372</v>
+        <v>376</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>374</v>
+        <v>378</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>376</v>
+        <v>380</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>378</v>
+        <v>382</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>380</v>
+        <v>384</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>382</v>
+        <v>386</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>384</v>
+        <v>388</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>386</v>
+        <v>390</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>388</v>
+        <v>392</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>390</v>
+        <v>394</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>392</v>
+        <v>396</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>394</v>
+        <v>398</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>396</v>
+        <v>400</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>398</v>
+        <v>402</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>400</v>
+        <v>404</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>405</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>407</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>408</v>
       </c>
     </row>
   </sheetData>
@@ -3567,138 +3635,138 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>402</v>
+        <v>410</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>403</v>
+        <v>411</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>404</v>
+        <v>412</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>405</v>
+        <v>413</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>406</v>
+        <v>414</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>407</v>
+        <v>415</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>408</v>
+        <v>416</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>409</v>
+        <v>417</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>410</v>
+        <v>418</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>411</v>
+        <v>419</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>412</v>
+        <v>420</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>413</v>
+        <v>421</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>414</v>
+        <v>422</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>415</v>
+        <v>423</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>416</v>
+        <v>424</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>417</v>
+        <v>425</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>387</v>
+        <v>395</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>388</v>
+        <v>396</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>418</v>
+        <v>426</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>419</v>
+        <v>427</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>420</v>
+        <v>428</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>421</v>
+        <v>429</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>422</v>
+        <v>430</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>423</v>
+        <v>431</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>424</v>
+        <v>432</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>425</v>
+        <v>433</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>426</v>
+        <v>434</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>427</v>
+        <v>435</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>428</v>
+        <v>436</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>429</v>
+        <v>437</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>430</v>
+        <v>438</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>431</v>
+        <v>439</v>
       </c>
     </row>
   </sheetData>
@@ -3716,12 +3784,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -3739,202 +3807,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>436</v>
+        <v>444</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>437</v>
+        <v>445</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>438</v>
+        <v>446</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>439</v>
+        <v>447</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>440</v>
+        <v>448</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>441</v>
+        <v>449</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>442</v>
+        <v>450</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>443</v>
+        <v>451</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>444</v>
+        <v>452</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>445</v>
+        <v>453</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>446</v>
+        <v>454</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>447</v>
+        <v>455</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>448</v>
+        <v>456</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>449</v>
+        <v>457</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>450</v>
+        <v>458</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>451</v>
+        <v>459</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>452</v>
+        <v>460</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>453</v>
+        <v>461</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>454</v>
+        <v>462</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>455</v>
+        <v>463</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>456</v>
+        <v>464</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>457</v>
+        <v>465</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>458</v>
+        <v>466</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>459</v>
+        <v>467</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>460</v>
+        <v>468</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>461</v>
+        <v>469</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>462</v>
+        <v>470</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>463</v>
+        <v>471</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>387</v>
+        <v>395</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>388</v>
+        <v>396</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>464</v>
+        <v>472</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>465</v>
+        <v>473</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>466</v>
+        <v>474</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>467</v>
+        <v>475</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>468</v>
+        <v>476</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>469</v>
+        <v>477</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>470</v>
+        <v>478</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>471</v>
+        <v>479</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>472</v>
+        <v>480</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>473</v>
+        <v>481</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>474</v>
+        <v>482</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>475</v>
+        <v>483</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>476</v>
+        <v>484</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>477</v>
+        <v>485</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>478</v>
+        <v>486</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>479</v>
+        <v>487</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>480</v>
+        <v>488</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>481</v>
+        <v>489</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>482</v>
+        <v>490</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>483</v>
+        <v>491</v>
       </c>
     </row>
   </sheetData>
@@ -3952,74 +4020,74 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>488</v>
+        <v>496</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>489</v>
+        <v>497</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>490</v>
+        <v>498</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>491</v>
+        <v>499</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>492</v>
+        <v>500</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>493</v>
+        <v>501</v>
       </c>
     </row>
   </sheetData>
@@ -4037,146 +4105,146 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>495</v>
+        <v>503</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>496</v>
+        <v>504</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>497</v>
+        <v>505</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>498</v>
+        <v>506</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>499</v>
+        <v>507</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>500</v>
+        <v>508</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>501</v>
+        <v>509</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>502</v>
+        <v>510</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>503</v>
+        <v>511</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>504</v>
+        <v>512</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>505</v>
+        <v>513</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>506</v>
+        <v>514</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>507</v>
+        <v>515</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>508</v>
+        <v>516</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>509</v>
+        <v>517</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>510</v>
+        <v>518</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>511</v>
+        <v>519</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>512</v>
+        <v>520</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>513</v>
+        <v>521</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>514</v>
+        <v>522</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>515</v>
+        <v>523</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>516</v>
+        <v>524</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>517</v>
+        <v>525</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>518</v>
+        <v>526</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>519</v>
+        <v>527</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>520</v>
+        <v>528</v>
       </c>
     </row>
   </sheetData>
@@ -4186,7 +4254,7 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4194,82 +4262,90 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>522</v>
+        <v>530</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>523</v>
+        <v>531</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>524</v>
+        <v>532</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>525</v>
+        <v>533</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>395</v>
+        <v>403</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>396</v>
+        <v>404</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>383</v>
+        <v>391</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>384</v>
+        <v>392</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>526</v>
+        <v>534</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>527</v>
+        <v>535</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>528</v>
+        <v>536</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>529</v>
+        <v>537</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>530</v>
+        <v>538</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>531</v>
+        <v>539</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>387</v>
+        <v>540</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>388</v>
+        <v>541</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>532</v>
+        <v>395</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>533</v>
+        <v>396</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>534</v>
+        <v>542</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>535</v>
+        <v>543</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>544</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>545</v>
       </c>
     </row>
   </sheetData>
@@ -4287,18 +4363,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -4308,7 +4384,7 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4316,98 +4392,106 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>539</v>
+        <v>549</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>540</v>
+        <v>550</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>541</v>
+        <v>551</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>542</v>
+        <v>552</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>543</v>
+        <v>553</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>544</v>
+        <v>554</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>545</v>
+        <v>555</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>546</v>
+        <v>556</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>547</v>
+        <v>395</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>548</v>
+        <v>396</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>549</v>
+        <v>557</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>550</v>
+        <v>558</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>551</v>
+        <v>559</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>552</v>
+        <v>560</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>387</v>
+        <v>561</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>388</v>
+        <v>562</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>553</v>
+        <v>563</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>554</v>
+        <v>564</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>555</v>
+        <v>565</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>556</v>
+        <v>566</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>557</v>
+        <v>567</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>558</v>
+        <v>568</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>559</v>
+        <v>569</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>560</v>
+        <v>570</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>571</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>572</v>
       </c>
     </row>
   </sheetData>
@@ -4425,122 +4509,122 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -4558,12 +4642,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -4587,30 +4671,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>564</v>
+        <v>576</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>565</v>
+        <v>577</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>567</v>
+        <v>579</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>569</v>
+        <v>581</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>566</v>
+        <v>578</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>568</v>
+        <v>580</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>570</v>
+        <v>582</v>
       </c>
     </row>
   </sheetData>
@@ -4628,12 +4712,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -4651,186 +4735,186 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -4848,418 +4932,418 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>213</v>
+        <v>217</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>219</v>
+        <v>223</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>223</v>
+        <v>227</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>225</v>
+        <v>229</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>227</v>
+        <v>231</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>231</v>
+        <v>235</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>233</v>
+        <v>237</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>235</v>
+        <v>239</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>239</v>
+        <v>243</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>241</v>
+        <v>245</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>257</v>
+        <v>261</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -5277,42 +5361,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>267</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -5330,26 +5414,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>267</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -5367,37 +5451,37 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>279</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>281</v>
+        <v>285</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>282</v>
+        <v>286</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>283</v>
+        <v>287</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>284</v>
+        <v>288</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Element Biosciences and its product AVITI and reagent kit
Closes #72, #73
</commit_message>
<xml_diff>
--- a/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
+++ b/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
@@ -416,7 +416,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="585">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="599">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -658,6 +658,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000207</t>
   </si>
   <si>
+    <t>MS Lipidomics</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000405</t>
+  </si>
+  <si>
     <t>analyte_class</t>
   </si>
   <si>
@@ -805,6 +811,12 @@
     <t>https://identifiers.org/RRID:SCR_023607</t>
   </si>
   <si>
+    <t>Vizgen</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026274</t>
+  </si>
+  <si>
     <t>Standard BioTools (Fluidigm)</t>
   </si>
   <si>
@@ -1162,6 +1174,12 @@
     <t>https://identifiers.org/RRID:SCR_023618</t>
   </si>
   <si>
+    <t>MERSCOPE</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000404</t>
+  </si>
+  <si>
     <t>NextSeq 2000</t>
   </si>
   <si>
@@ -1204,6 +1222,12 @@
     <t>https://identifiers.org/RRID:SCR_023909</t>
   </si>
   <si>
+    <t>MERSCOPE Ultra</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026273</t>
+  </si>
+  <si>
     <t>Axio Scan.Z1</t>
   </si>
   <si>
@@ -1792,6 +1816,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000283</t>
   </si>
   <si>
+    <t>Element Biosciences; AVITI 2x75 Sequencing Kit Cloudbreak FS High Output (184 Cycles); PN 860-00015</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000406</t>
+  </si>
+  <si>
     <t>Illumina; NovaSeq X Series 1.5B Reagent Kit (100 Cycle); PN 20104703</t>
   </si>
   <si>
@@ -1924,6 +1954,12 @@
     <t>https://identifiers.org/RRID:SCR_023734</t>
   </si>
   <si>
+    <t>Element Biosciences</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026453</t>
+  </si>
+  <si>
     <t>SunChrom</t>
   </si>
   <si>
@@ -1963,6 +1999,12 @@
     <t>https://identifiers.org/RRID:SCR_024570</t>
   </si>
   <si>
+    <t>AVITI</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026452</t>
+  </si>
+  <si>
     <t>SunCollect Sprayer</t>
   </si>
   <si>
@@ -2164,7 +2206,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-01-08T12:44:31-08:00</t>
+    <t>2025-02-21T09:59:41-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -2364,148 +2406,148 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>291</v>
+        <v>299</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>323</v>
+        <v>331</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>324</v>
+        <v>332</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>329</v>
+        <v>337</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>330</v>
+        <v>338</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>331</v>
+        <v>339</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>332</v>
+        <v>340</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>335</v>
+        <v>343</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>336</v>
+        <v>344</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>337</v>
+        <v>345</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>338</v>
+        <v>346</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>348</v>
+        <v>356</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>349</v>
+        <v>357</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>350</v>
+        <v>358</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>411</v>
+        <v>419</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>442</v>
+        <v>450</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>443</v>
+        <v>451</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>444</v>
+        <v>452</v>
       </c>
       <c r="AO1" t="s" s="1">
-        <v>445</v>
+        <v>453</v>
       </c>
       <c r="AP1" t="s" s="1">
-        <v>494</v>
+        <v>504</v>
       </c>
       <c r="AQ1" t="s" s="1">
-        <v>495</v>
+        <v>505</v>
       </c>
       <c r="AR1" t="s" s="1">
-        <v>496</v>
+        <v>506</v>
       </c>
       <c r="AS1" t="s" s="1">
-        <v>497</v>
+        <v>507</v>
       </c>
       <c r="AT1" t="s" s="1">
-        <v>504</v>
+        <v>516</v>
       </c>
       <c r="AU1" t="s" s="1">
-        <v>531</v>
+        <v>545</v>
       </c>
       <c r="AV1" t="s" s="1">
-        <v>548</v>
+        <v>562</v>
       </c>
       <c r="AW1" t="s" s="1">
-        <v>549</v>
+        <v>563</v>
       </c>
       <c r="AX1" t="s" s="1">
-        <v>550</v>
+        <v>564</v>
       </c>
       <c r="AY1" t="s" s="1">
-        <v>575</v>
+        <v>589</v>
       </c>
       <c r="AZ1" t="s" s="1">
-        <v>576</v>
+        <v>590</v>
       </c>
     </row>
     <row r="2">
@@ -2513,13 +2555,13 @@
         <v>72</v>
       </c>
       <c r="AZ2" t="s" s="53">
-        <v>577</v>
+        <v>591</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="41">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$38</formula1>
+      <formula1>'dataset_type'!$A$1:$A$39</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'analyte_class'!$A$1:$A$16</formula1>
@@ -2528,10 +2570,10 @@
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$23</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$24</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$52</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$54</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -2629,13 +2671,13 @@
       <formula2>2147483647</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="AO2:AO1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'sequencing_reagent_kit'!$A$1:$A$25</formula1>
+      <formula1>'sequencing_reagent_kit'!$A$1:$A$26</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AS2:AS1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_instrument_vendor'!$A$1:$A$9</formula1>
+      <formula1>'preparation_instrument_vendor'!$A$1:$A$10</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AT2:AT1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_instrument_model'!$A$1:$A$18</formula1>
+      <formula1>'preparation_instrument_model'!$A$1:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AU2:AU1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'preparation_instrument_kit'!$A$1:$A$11</formula1>
@@ -2670,26 +2712,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>292</v>
+        <v>300</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>293</v>
+        <v>301</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>295</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -2707,37 +2749,37 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>297</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>298</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>299</v>
+        <v>307</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>300</v>
+        <v>308</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>301</v>
+        <v>309</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>302</v>
+        <v>310</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -2755,27 +2797,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>285</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>298</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>304</v>
+        <v>312</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>305</v>
+        <v>313</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -2793,26 +2835,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>292</v>
+        <v>300</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>293</v>
+        <v>301</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>295</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -2830,32 +2872,32 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>286</v>
+        <v>294</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>308</v>
+        <v>316</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>309</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>310</v>
+        <v>318</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>297</v>
+        <v>305</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -2873,42 +2915,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>313</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>315</v>
+        <v>323</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>316</v>
+        <v>324</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>317</v>
+        <v>325</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>319</v>
+        <v>327</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>321</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -2926,18 +2968,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>325</v>
+        <v>333</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>326</v>
+        <v>334</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>327</v>
+        <v>335</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>328</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -2955,18 +2997,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>334</v>
+        <v>342</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>327</v>
+        <v>335</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>328</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -2984,18 +3026,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>334</v>
+        <v>342</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>327</v>
+        <v>335</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>328</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -3013,18 +3055,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>339</v>
+        <v>347</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>340</v>
+        <v>348</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>341</v>
+        <v>349</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>342</v>
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -3034,7 +3076,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3342,6 +3384,14 @@
       </c>
       <c r="B38" t="s" s="0">
         <v>79</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="B39" t="s" s="0">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -3359,18 +3409,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>344</v>
+        <v>352</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>345</v>
+        <v>353</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>346</v>
+        <v>354</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>347</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>
@@ -3388,242 +3438,242 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>351</v>
+        <v>359</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>352</v>
+        <v>360</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>353</v>
+        <v>361</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>354</v>
+        <v>362</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>355</v>
+        <v>363</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>356</v>
+        <v>364</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>357</v>
+        <v>365</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>358</v>
+        <v>366</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>359</v>
+        <v>367</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>360</v>
+        <v>368</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>361</v>
+        <v>369</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>362</v>
+        <v>370</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>363</v>
+        <v>371</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>364</v>
+        <v>372</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>365</v>
+        <v>373</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>366</v>
+        <v>374</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>367</v>
+        <v>375</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>368</v>
+        <v>376</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>369</v>
+        <v>377</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>370</v>
+        <v>378</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>371</v>
+        <v>379</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>372</v>
+        <v>380</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>373</v>
+        <v>381</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>374</v>
+        <v>382</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>375</v>
+        <v>383</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>376</v>
+        <v>384</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>377</v>
+        <v>385</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>378</v>
+        <v>386</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>379</v>
+        <v>387</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>380</v>
+        <v>388</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>381</v>
+        <v>389</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>382</v>
+        <v>390</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>383</v>
+        <v>391</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>384</v>
+        <v>392</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>385</v>
+        <v>393</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>386</v>
+        <v>394</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>387</v>
+        <v>395</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>388</v>
+        <v>396</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>389</v>
+        <v>397</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>390</v>
+        <v>398</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>391</v>
+        <v>399</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>392</v>
+        <v>400</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>393</v>
+        <v>401</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>394</v>
+        <v>402</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>395</v>
+        <v>403</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>396</v>
+        <v>404</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>397</v>
+        <v>405</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>398</v>
+        <v>406</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>399</v>
+        <v>407</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>400</v>
+        <v>408</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>401</v>
+        <v>409</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>402</v>
+        <v>410</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>403</v>
+        <v>411</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>404</v>
+        <v>412</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>405</v>
+        <v>413</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>406</v>
+        <v>414</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>407</v>
+        <v>415</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>408</v>
+        <v>416</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>409</v>
+        <v>417</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>410</v>
+        <v>418</v>
       </c>
     </row>
   </sheetData>
@@ -3641,138 +3691,138 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>412</v>
+        <v>420</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>413</v>
+        <v>421</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>414</v>
+        <v>422</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>415</v>
+        <v>423</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>416</v>
+        <v>424</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>417</v>
+        <v>425</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>418</v>
+        <v>426</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>419</v>
+        <v>427</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>420</v>
+        <v>428</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>421</v>
+        <v>429</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>422</v>
+        <v>430</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>423</v>
+        <v>431</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>424</v>
+        <v>432</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>425</v>
+        <v>433</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>426</v>
+        <v>434</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>427</v>
+        <v>435</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>397</v>
+        <v>405</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>398</v>
+        <v>406</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>428</v>
+        <v>436</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>429</v>
+        <v>437</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>430</v>
+        <v>438</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>431</v>
+        <v>439</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>433</v>
+        <v>441</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>435</v>
+        <v>443</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>436</v>
+        <v>444</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>437</v>
+        <v>445</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>438</v>
+        <v>446</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>439</v>
+        <v>447</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>440</v>
+        <v>448</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>441</v>
+        <v>449</v>
       </c>
     </row>
   </sheetData>
@@ -3790,12 +3840,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -3805,7 +3855,7 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3813,202 +3863,210 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>446</v>
+        <v>454</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>447</v>
+        <v>455</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>448</v>
+        <v>456</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>449</v>
+        <v>457</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>450</v>
+        <v>458</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>451</v>
+        <v>459</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>452</v>
+        <v>460</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>453</v>
+        <v>461</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>454</v>
+        <v>462</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>455</v>
+        <v>463</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>456</v>
+        <v>464</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>457</v>
+        <v>465</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>458</v>
+        <v>466</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>459</v>
+        <v>467</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>460</v>
+        <v>468</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>461</v>
+        <v>469</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>462</v>
+        <v>470</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>463</v>
+        <v>471</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>464</v>
+        <v>472</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>465</v>
+        <v>473</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>466</v>
+        <v>474</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>467</v>
+        <v>475</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>468</v>
+        <v>476</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>469</v>
+        <v>477</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>470</v>
+        <v>478</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>471</v>
+        <v>479</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>472</v>
+        <v>480</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>473</v>
+        <v>481</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>397</v>
+        <v>482</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>398</v>
+        <v>483</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>474</v>
+        <v>405</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>475</v>
+        <v>406</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>476</v>
+        <v>484</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>477</v>
+        <v>485</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>478</v>
+        <v>486</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>479</v>
+        <v>487</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>480</v>
+        <v>488</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>481</v>
+        <v>489</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>482</v>
+        <v>490</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>483</v>
+        <v>491</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>484</v>
+        <v>492</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>485</v>
+        <v>493</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>486</v>
+        <v>494</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>487</v>
+        <v>495</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>488</v>
+        <v>496</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>489</v>
+        <v>497</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>490</v>
+        <v>498</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>491</v>
+        <v>499</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>492</v>
+        <v>500</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>493</v>
+        <v>501</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>502</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>503</v>
       </c>
     </row>
   </sheetData>
@@ -4018,7 +4076,7 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4026,74 +4084,82 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>498</v>
+        <v>508</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>499</v>
+        <v>509</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>500</v>
+        <v>510</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>501</v>
+        <v>511</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>151</v>
+        <v>512</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>152</v>
+        <v>513</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>502</v>
+        <v>155</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>503</v>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>514</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>515</v>
       </c>
     </row>
   </sheetData>
@@ -4103,7 +4169,7 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4111,146 +4177,154 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>505</v>
+        <v>517</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>506</v>
+        <v>518</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>507</v>
+        <v>519</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>508</v>
+        <v>520</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>259</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>509</v>
+        <v>521</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>510</v>
+        <v>522</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>511</v>
+        <v>523</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>512</v>
+        <v>524</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>513</v>
+        <v>525</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>514</v>
+        <v>526</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>515</v>
+        <v>527</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>516</v>
+        <v>528</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>517</v>
+        <v>529</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>518</v>
+        <v>530</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>520</v>
+        <v>532</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>521</v>
+        <v>533</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>522</v>
+        <v>534</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>523</v>
+        <v>535</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>524</v>
+        <v>536</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>525</v>
+        <v>537</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>526</v>
+        <v>538</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>527</v>
+        <v>539</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>528</v>
+        <v>540</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>529</v>
+        <v>541</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>530</v>
+        <v>542</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>543</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>544</v>
       </c>
     </row>
   </sheetData>
@@ -4268,90 +4342,90 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>532</v>
+        <v>546</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>533</v>
+        <v>547</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>534</v>
+        <v>548</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>535</v>
+        <v>549</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>405</v>
+        <v>413</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>406</v>
+        <v>414</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>393</v>
+        <v>401</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>394</v>
+        <v>402</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>536</v>
+        <v>550</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>537</v>
+        <v>551</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>538</v>
+        <v>552</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>539</v>
+        <v>553</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>540</v>
+        <v>554</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>541</v>
+        <v>555</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>542</v>
+        <v>556</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>543</v>
+        <v>557</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>397</v>
+        <v>405</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>398</v>
+        <v>406</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>544</v>
+        <v>558</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>545</v>
+        <v>559</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>546</v>
+        <v>560</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>547</v>
+        <v>561</v>
       </c>
     </row>
   </sheetData>
@@ -4369,18 +4443,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>271</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>279</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -4398,106 +4472,106 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>551</v>
+        <v>565</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>552</v>
+        <v>566</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>553</v>
+        <v>567</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>554</v>
+        <v>568</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>555</v>
+        <v>569</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>556</v>
+        <v>570</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>557</v>
+        <v>571</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>558</v>
+        <v>572</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>397</v>
+        <v>405</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>398</v>
+        <v>406</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>559</v>
+        <v>573</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>560</v>
+        <v>574</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>561</v>
+        <v>575</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>562</v>
+        <v>576</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>563</v>
+        <v>577</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>564</v>
+        <v>578</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>565</v>
+        <v>579</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>566</v>
+        <v>580</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>567</v>
+        <v>581</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>568</v>
+        <v>582</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>569</v>
+        <v>583</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>570</v>
+        <v>584</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>571</v>
+        <v>585</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>572</v>
+        <v>586</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>573</v>
+        <v>587</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>574</v>
+        <v>588</v>
       </c>
     </row>
   </sheetData>
@@ -4515,130 +4589,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -4656,12 +4730,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -4685,16 +4759,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>578</v>
+        <v>592</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>579</v>
+        <v>593</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>581</v>
+        <v>595</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>583</v>
+        <v>597</v>
       </c>
     </row>
     <row r="2">
@@ -4702,13 +4776,13 @@
         <v>72</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>580</v>
+        <v>594</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>582</v>
+        <v>596</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>584</v>
+        <v>598</v>
       </c>
     </row>
   </sheetData>
@@ -4726,12 +4800,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -4741,7 +4815,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4749,186 +4823,194 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -4938,7 +5020,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4946,418 +5028,434 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>213</v>
+        <v>217</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>219</v>
+        <v>223</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>223</v>
+        <v>227</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>225</v>
+        <v>229</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>227</v>
+        <v>231</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>231</v>
+        <v>235</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>233</v>
+        <v>237</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>235</v>
+        <v>239</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>239</v>
+        <v>243</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>241</v>
+        <v>245</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>257</v>
+        <v>261</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>267</v>
+        <v>271</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="0">
+        <v>272</v>
+      </c>
+      <c r="B53" t="s" s="0">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="0">
+        <v>274</v>
+      </c>
+      <c r="B54" t="s" s="0">
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -5375,42 +5473,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>271</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>273</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>275</v>
+        <v>283</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>276</v>
+        <v>284</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>277</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>279</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -5428,26 +5526,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>273</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>275</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>276</v>
+        <v>284</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>277</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -5465,37 +5563,37 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>285</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>286</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>287</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>288</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>289</v>
+        <v>297</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>290</v>
+        <v>298</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a new oligo probe panel and library preparation kit
Closes #84
</commit_message>
<xml_diff>
--- a/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
+++ b/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
@@ -416,7 +416,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="621">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="633">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -502,10 +502,10 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000218</t>
   </si>
   <si>
-    <t>DBiT</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000222</t>
+    <t>DBiT-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
   </si>
   <si>
     <t>SIMS</t>
@@ -604,6 +604,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000310</t>
   </si>
   <si>
+    <t>Singular Genomics G4X</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000429</t>
+  </si>
+  <si>
     <t>MERFISH</t>
   </si>
   <si>
@@ -871,6 +877,12 @@
     <t>https://identifiers.org/RRID:SCR_023911</t>
   </si>
   <si>
+    <t>Singular Genomics</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026683</t>
+  </si>
+  <si>
     <t>Vizgen</t>
   </si>
   <si>
@@ -1090,6 +1102,12 @@
     <t>https://identifiers.org/RRID:SCR_026551</t>
   </si>
   <si>
+    <t>G4X Spatial Sequencer</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026684</t>
+  </si>
+  <si>
     <t>NextSeq 500</t>
   </si>
   <si>
@@ -1615,6 +1633,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000399</t>
   </si>
   <si>
+    <t>10x Genomics; Visium CytAssist Spatial Gene Expression for FFPE, Mouse Transcriptome, 6.5mm, 4 rxns; PN 1000521</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000432</t>
+  </si>
+  <si>
     <t>10X Genomics; Chromium Next GEM Single Cell 3' HT Kit v3.1, 48 rxns; PN 1000348</t>
   </si>
   <si>
@@ -2203,6 +2227,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000326</t>
   </si>
   <si>
+    <t>10x Genomics; Visium Mouse Transcriptome Probe Kit v2.0 - Small; PN 1000667</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000431</t>
+  </si>
+  <si>
     <t>NanoString Technologies; GeoMx Human Whole Transcriptome Atlas, 4 slides; PN GMX-RNA-NGS-HuWTA-4</t>
   </si>
   <si>
@@ -2245,6 +2275,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000362</t>
   </si>
   <si>
+    <t>NanoString Technologies; CosMx Human Universal Cell Characterization Panel (RNA, 1000 Plex); PN CMX-H-USCP-1KP-R</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000430</t>
+  </si>
+  <si>
     <t>10X Genomics; Chromium Next GEM Single Cell Fixed RNA Human Transcriptome Probe Kit, 16 rxns; PN 1000420</t>
   </si>
   <si>
@@ -2272,7 +2308,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-03-27T10:50:44-07:00</t>
+    <t>2025-04-15T09:51:38-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -2472,162 +2508,162 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>315</v>
+        <v>321</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>338</v>
+        <v>344</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>343</v>
+        <v>349</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>354</v>
+        <v>360</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>355</v>
+        <v>361</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>356</v>
+        <v>362</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>443</v>
+        <v>451</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>474</v>
+        <v>482</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>475</v>
+        <v>483</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>476</v>
+        <v>484</v>
       </c>
       <c r="AO1" t="s" s="1">
-        <v>477</v>
+        <v>485</v>
       </c>
       <c r="AP1" t="s" s="1">
-        <v>528</v>
+        <v>536</v>
       </c>
       <c r="AQ1" t="s" s="1">
-        <v>529</v>
+        <v>537</v>
       </c>
       <c r="AR1" t="s" s="1">
-        <v>530</v>
+        <v>538</v>
       </c>
       <c r="AS1" t="s" s="1">
-        <v>531</v>
+        <v>539</v>
       </c>
       <c r="AT1" t="s" s="1">
-        <v>538</v>
+        <v>546</v>
       </c>
       <c r="AU1" t="s" s="1">
-        <v>565</v>
+        <v>573</v>
       </c>
       <c r="AV1" t="s" s="1">
-        <v>582</v>
+        <v>590</v>
       </c>
       <c r="AW1" t="s" s="1">
-        <v>583</v>
+        <v>591</v>
       </c>
       <c r="AX1" t="s" s="1">
-        <v>584</v>
+        <v>592</v>
       </c>
       <c r="AY1" t="s" s="1">
-        <v>611</v>
+        <v>623</v>
       </c>
       <c r="AZ1" t="s" s="1">
-        <v>612</v>
+        <v>624</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="AZ2" t="s" s="53">
-        <v>613</v>
+        <v>625</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="41">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$40</formula1>
+      <formula1>'dataset_type'!$A$1:$A$41</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'analyte_class'!$A$1:$A$16</formula1>
@@ -2636,10 +2672,10 @@
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$25</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$26</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$64</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$66</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -2724,7 +2760,7 @@
       <formula2>2147483647</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="AJ2:AJ1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'library_preparation_kit'!$A$1:$A$30</formula1>
+      <formula1>'library_preparation_kit'!$A$1:$A$31</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AK2:AK1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'sample_indexing_kit'!$A$1:$A$17</formula1>
@@ -2756,7 +2792,7 @@
       <formula1>'probe_hybridization_time_unit'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AX2:AX1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'oligo_probe_panel'!$A$1:$A$14</formula1>
+      <formula1>'oligo_probe_panel'!$A$1:$A$16</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AY2:AY1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_custom_probes_used'!$A$1:$A$2</formula1>
@@ -2778,26 +2814,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>325</v>
+        <v>331</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>327</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -2815,37 +2851,37 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>329</v>
+        <v>335</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>330</v>
+        <v>336</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>331</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>332</v>
+        <v>338</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>333</v>
+        <v>339</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>334</v>
+        <v>340</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -2863,27 +2899,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>317</v>
+        <v>323</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>330</v>
+        <v>336</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>336</v>
+        <v>342</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>337</v>
+        <v>343</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -2901,26 +2937,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>325</v>
+        <v>331</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>327</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -2938,32 +2974,32 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>318</v>
+        <v>324</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>340</v>
+        <v>346</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>341</v>
+        <v>347</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>342</v>
+        <v>348</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>329</v>
+        <v>335</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -2981,42 +3017,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>344</v>
+        <v>350</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>345</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>346</v>
+        <v>352</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>347</v>
+        <v>353</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>348</v>
+        <v>354</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>349</v>
+        <v>355</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>350</v>
+        <v>356</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>351</v>
+        <v>357</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>353</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -3034,18 +3070,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>357</v>
+        <v>363</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>358</v>
+        <v>364</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>360</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -3063,18 +3099,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>366</v>
+        <v>372</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>360</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -3092,18 +3128,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>366</v>
+        <v>372</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>360</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -3121,18 +3157,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>372</v>
+        <v>378</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>373</v>
+        <v>379</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>374</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>
@@ -3142,7 +3178,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3466,6 +3502,14 @@
       </c>
       <c r="B40" t="s" s="0">
         <v>83</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="B41" t="s" s="0">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -3483,18 +3527,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>377</v>
+        <v>383</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>379</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>
@@ -3504,7 +3548,7 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3512,242 +3556,250 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>384</v>
+        <v>390</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>386</v>
+        <v>392</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>388</v>
+        <v>394</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>390</v>
+        <v>396</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>391</v>
+        <v>397</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>392</v>
+        <v>398</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>394</v>
+        <v>400</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>395</v>
+        <v>401</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>396</v>
+        <v>402</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>398</v>
+        <v>404</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>399</v>
+        <v>405</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>400</v>
+        <v>406</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>401</v>
+        <v>407</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>402</v>
+        <v>408</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>403</v>
+        <v>409</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>405</v>
+        <v>411</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>406</v>
+        <v>412</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>407</v>
+        <v>413</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>408</v>
+        <v>414</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>410</v>
+        <v>416</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>411</v>
+        <v>417</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>412</v>
+        <v>418</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>413</v>
+        <v>419</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>414</v>
+        <v>420</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>415</v>
+        <v>421</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>416</v>
+        <v>422</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>417</v>
+        <v>423</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>418</v>
+        <v>424</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>419</v>
+        <v>425</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>420</v>
+        <v>426</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>421</v>
+        <v>427</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>422</v>
+        <v>428</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>423</v>
+        <v>429</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>424</v>
+        <v>430</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>426</v>
+        <v>432</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>427</v>
+        <v>433</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>428</v>
+        <v>434</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>429</v>
+        <v>435</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>430</v>
+        <v>436</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>431</v>
+        <v>437</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>432</v>
+        <v>438</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>433</v>
+        <v>439</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>434</v>
+        <v>440</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>435</v>
+        <v>441</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>436</v>
+        <v>442</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>438</v>
+        <v>444</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>439</v>
+        <v>445</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>440</v>
+        <v>446</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>442</v>
+        <v>448</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>449</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>450</v>
       </c>
     </row>
   </sheetData>
@@ -3765,138 +3817,138 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>444</v>
+        <v>452</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>445</v>
+        <v>453</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>446</v>
+        <v>454</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>447</v>
+        <v>455</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>448</v>
+        <v>456</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>449</v>
+        <v>457</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>450</v>
+        <v>458</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>451</v>
+        <v>459</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>452</v>
+        <v>460</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>453</v>
+        <v>461</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>454</v>
+        <v>462</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>455</v>
+        <v>463</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>456</v>
+        <v>464</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>457</v>
+        <v>465</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>458</v>
+        <v>466</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>459</v>
+        <v>467</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>429</v>
+        <v>437</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>430</v>
+        <v>438</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>460</v>
+        <v>468</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>461</v>
+        <v>469</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>462</v>
+        <v>470</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>463</v>
+        <v>471</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>464</v>
+        <v>472</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>465</v>
+        <v>473</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>466</v>
+        <v>474</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>467</v>
+        <v>475</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>468</v>
+        <v>476</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>469</v>
+        <v>477</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>470</v>
+        <v>478</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>471</v>
+        <v>479</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>472</v>
+        <v>480</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>473</v>
+        <v>481</v>
       </c>
     </row>
   </sheetData>
@@ -3914,12 +3966,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -3937,210 +3989,210 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>478</v>
+        <v>486</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>479</v>
+        <v>487</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>480</v>
+        <v>488</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>481</v>
+        <v>489</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>482</v>
+        <v>490</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>483</v>
+        <v>491</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>484</v>
+        <v>492</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>485</v>
+        <v>493</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>486</v>
+        <v>494</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>487</v>
+        <v>495</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>488</v>
+        <v>496</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>489</v>
+        <v>497</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>490</v>
+        <v>498</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>491</v>
+        <v>499</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>492</v>
+        <v>500</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>493</v>
+        <v>501</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>494</v>
+        <v>502</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>495</v>
+        <v>503</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>496</v>
+        <v>504</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>497</v>
+        <v>505</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>498</v>
+        <v>506</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>499</v>
+        <v>507</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>500</v>
+        <v>508</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>501</v>
+        <v>509</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>502</v>
+        <v>510</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>503</v>
+        <v>511</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>504</v>
+        <v>512</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>505</v>
+        <v>513</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>506</v>
+        <v>514</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>507</v>
+        <v>515</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>429</v>
+        <v>437</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>430</v>
+        <v>438</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>508</v>
+        <v>516</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>509</v>
+        <v>517</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>510</v>
+        <v>518</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>511</v>
+        <v>519</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>512</v>
+        <v>520</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>513</v>
+        <v>521</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>514</v>
+        <v>522</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>515</v>
+        <v>523</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>516</v>
+        <v>524</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>517</v>
+        <v>525</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>518</v>
+        <v>526</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>519</v>
+        <v>527</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>520</v>
+        <v>528</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>521</v>
+        <v>529</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>522</v>
+        <v>530</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>523</v>
+        <v>531</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>524</v>
+        <v>532</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>525</v>
+        <v>533</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>526</v>
+        <v>534</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>527</v>
+        <v>535</v>
       </c>
     </row>
   </sheetData>
@@ -4158,74 +4210,74 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>532</v>
+        <v>540</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>533</v>
+        <v>541</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>534</v>
+        <v>542</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>535</v>
+        <v>543</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>536</v>
+        <v>544</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>537</v>
+        <v>545</v>
       </c>
     </row>
   </sheetData>
@@ -4243,146 +4295,146 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>539</v>
+        <v>547</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>540</v>
+        <v>548</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>541</v>
+        <v>549</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>542</v>
+        <v>550</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>289</v>
+        <v>295</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>543</v>
+        <v>551</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>544</v>
+        <v>552</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>545</v>
+        <v>553</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>546</v>
+        <v>554</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>547</v>
+        <v>555</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>548</v>
+        <v>556</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>549</v>
+        <v>557</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>550</v>
+        <v>558</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>551</v>
+        <v>559</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>552</v>
+        <v>560</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>553</v>
+        <v>561</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>554</v>
+        <v>562</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>555</v>
+        <v>563</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>556</v>
+        <v>564</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>557</v>
+        <v>565</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>558</v>
+        <v>566</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>559</v>
+        <v>567</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>560</v>
+        <v>568</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>561</v>
+        <v>569</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>562</v>
+        <v>570</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>563</v>
+        <v>571</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>564</v>
+        <v>572</v>
       </c>
     </row>
   </sheetData>
@@ -4400,90 +4452,90 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>566</v>
+        <v>574</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>567</v>
+        <v>575</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>568</v>
+        <v>576</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>569</v>
+        <v>577</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>437</v>
+        <v>445</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>438</v>
+        <v>446</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>425</v>
+        <v>433</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>426</v>
+        <v>434</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>570</v>
+        <v>578</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>571</v>
+        <v>579</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>572</v>
+        <v>580</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>573</v>
+        <v>581</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>574</v>
+        <v>582</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>575</v>
+        <v>583</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>576</v>
+        <v>584</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>577</v>
+        <v>585</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>429</v>
+        <v>437</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>430</v>
+        <v>438</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>578</v>
+        <v>586</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>579</v>
+        <v>587</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>580</v>
+        <v>588</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>581</v>
+        <v>589</v>
       </c>
     </row>
   </sheetData>
@@ -4501,18 +4553,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>303</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>311</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -4522,7 +4574,7 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4530,114 +4582,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>585</v>
+        <v>593</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>586</v>
+        <v>594</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>587</v>
+        <v>595</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>588</v>
+        <v>596</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>589</v>
+        <v>597</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>590</v>
+        <v>598</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>591</v>
+        <v>599</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>592</v>
+        <v>600</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>593</v>
+        <v>601</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>594</v>
+        <v>602</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>429</v>
+        <v>603</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>430</v>
+        <v>604</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>595</v>
+        <v>437</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>596</v>
+        <v>438</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>597</v>
+        <v>605</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>598</v>
+        <v>606</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>599</v>
+        <v>607</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>600</v>
+        <v>608</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>601</v>
+        <v>609</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>602</v>
+        <v>610</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>604</v>
+        <v>612</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>605</v>
+        <v>613</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>606</v>
+        <v>614</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>607</v>
+        <v>615</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>608</v>
+        <v>616</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>609</v>
+        <v>617</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>610</v>
+        <v>618</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>619</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>621</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>622</v>
       </c>
     </row>
   </sheetData>
@@ -4655,130 +4723,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -4796,12 +4864,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -4825,30 +4893,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>614</v>
+        <v>626</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>615</v>
+        <v>627</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>617</v>
+        <v>629</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>619</v>
+        <v>631</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>616</v>
+        <v>628</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>618</v>
+        <v>630</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>620</v>
+        <v>632</v>
       </c>
     </row>
   </sheetData>
@@ -4866,12 +4934,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -4881,7 +4949,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4889,202 +4957,210 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>170</v>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>173</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -5094,7 +5170,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B64"/>
+  <dimension ref="A1:B66"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5102,514 +5178,530 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>213</v>
+        <v>217</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>219</v>
+        <v>223</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>223</v>
+        <v>227</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>225</v>
+        <v>229</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>227</v>
+        <v>231</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>231</v>
+        <v>235</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>233</v>
+        <v>237</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>235</v>
+        <v>239</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>239</v>
+        <v>243</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>241</v>
+        <v>245</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>257</v>
+        <v>261</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>267</v>
+        <v>271</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>275</v>
+        <v>279</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>279</v>
+        <v>283</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>281</v>
+        <v>285</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>283</v>
+        <v>287</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>284</v>
+        <v>149</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>285</v>
+        <v>150</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>299</v>
+        <v>301</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s" s="0">
+        <v>302</v>
+      </c>
+      <c r="B65" t="s" s="0">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s" s="0">
+        <v>304</v>
+      </c>
+      <c r="B66" t="s" s="0">
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -5627,42 +5719,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>303</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>307</v>
+        <v>313</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>309</v>
+        <v>315</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>311</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -5680,26 +5772,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>307</v>
+        <v>313</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>309</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -5717,37 +5809,37 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>317</v>
+        <v>323</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>318</v>
+        <v>324</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>319</v>
+        <v>325</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>320</v>
+        <v>326</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>321</v>
+        <v>327</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>322</v>
+        <v>328</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a new concentration unit
Closes #93
</commit_message>
<xml_diff>
--- a/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
+++ b/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
@@ -416,7 +416,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="647">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -574,6 +574,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000309</t>
   </si>
   <si>
+    <t>CosMx Proteomics</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000435</t>
+  </si>
+  <si>
     <t>Histology</t>
   </si>
   <si>
@@ -811,6 +817,12 @@
     <t>https://identifiers.org/RRID:SCR_023607</t>
   </si>
   <si>
+    <t>Complete Genomics</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027007</t>
+  </si>
+  <si>
     <t>GE Healthcare</t>
   </si>
   <si>
@@ -1567,6 +1579,12 @@
     <t>http://purl.obolibrary.org/obo/UO_0010050</t>
   </si>
   <si>
+    <t>pg/ul</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000438</t>
+  </si>
+  <si>
     <t>nM</t>
   </si>
   <si>
@@ -2275,6 +2293,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000376</t>
   </si>
   <si>
+    <t>NanoString Technologies; CosMx Human Immuno-Oncology Panel (Protein, 64 Plex); PN CMX-H-IOP-64P-P</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000436</t>
+  </si>
+  <si>
     <t>10x Genomics; Chromium Fixed RNA Kit, Human Transcriptome, 4 rxns x 1 BC; PN 1000474</t>
   </si>
   <si>
@@ -2293,6 +2317,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000430</t>
   </si>
   <si>
+    <t>NanoString Technologies; CosMx Mouse Neuroscience Panel (Protein, 64 Plex); PN CMX-M-Neuro-64P-P</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000437</t>
+  </si>
+  <si>
     <t>10X Genomics; Chromium Next GEM Single Cell Fixed RNA Human Transcriptome Probe Kit, 16 rxns; PN 1000420</t>
   </si>
   <si>
@@ -2320,7 +2350,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-05-12T10:15:37-07:00</t>
+    <t>2025-06-10T10:06:43-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -2520,162 +2550,162 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>391</v>
+        <v>397</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>392</v>
+        <v>398</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>455</v>
+        <v>461</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>486</v>
+        <v>492</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>487</v>
+        <v>493</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>488</v>
+        <v>494</v>
       </c>
       <c r="AO1" t="s" s="1">
-        <v>489</v>
+        <v>495</v>
       </c>
       <c r="AP1" t="s" s="1">
-        <v>540</v>
+        <v>546</v>
       </c>
       <c r="AQ1" t="s" s="1">
-        <v>541</v>
+        <v>547</v>
       </c>
       <c r="AR1" t="s" s="1">
-        <v>542</v>
+        <v>548</v>
       </c>
       <c r="AS1" t="s" s="1">
-        <v>543</v>
+        <v>549</v>
       </c>
       <c r="AT1" t="s" s="1">
-        <v>550</v>
+        <v>556</v>
       </c>
       <c r="AU1" t="s" s="1">
-        <v>577</v>
+        <v>583</v>
       </c>
       <c r="AV1" t="s" s="1">
-        <v>594</v>
+        <v>600</v>
       </c>
       <c r="AW1" t="s" s="1">
-        <v>595</v>
+        <v>601</v>
       </c>
       <c r="AX1" t="s" s="1">
-        <v>596</v>
+        <v>602</v>
       </c>
       <c r="AY1" t="s" s="1">
-        <v>627</v>
+        <v>637</v>
       </c>
       <c r="AZ1" t="s" s="1">
-        <v>628</v>
+        <v>638</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AZ2" t="s" s="53">
-        <v>629</v>
+        <v>639</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="41">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$41</formula1>
+      <formula1>'dataset_type'!$A$1:$A$42</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'analyte_class'!$A$1:$A$16</formula1>
@@ -2684,7 +2714,7 @@
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$26</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$27</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'acquisition_instrument_model'!$A$1:$A$68</formula1>
@@ -2758,7 +2788,7 @@
       <formula2>3.4028235E38</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="AF2:AF1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'library_concentration_unit'!$A$1:$A$2</formula1>
+      <formula1>'library_concentration_unit'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AG2:AG1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'library_layout'!$A$1:$A$2</formula1>
@@ -2804,7 +2834,7 @@
       <formula1>'probe_hybridization_time_unit'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AX2:AX1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'oligo_probe_panel'!$A$1:$A$16</formula1>
+      <formula1>'oligo_probe_panel'!$A$1:$A$18</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AY2:AY1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_custom_probes_used'!$A$1:$A$2</formula1>
@@ -2826,26 +2856,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>335</v>
+        <v>339</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>337</v>
+        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -2863,37 +2893,37 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>339</v>
+        <v>343</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>340</v>
+        <v>344</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>341</v>
+        <v>345</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>342</v>
+        <v>346</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>343</v>
+        <v>347</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>344</v>
+        <v>348</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -2911,27 +2941,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>327</v>
+        <v>331</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>340</v>
+        <v>344</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>346</v>
+        <v>350</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>347</v>
+        <v>351</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -2949,26 +2979,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>335</v>
+        <v>339</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>337</v>
+        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -2986,32 +3016,32 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>328</v>
+        <v>332</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>350</v>
+        <v>354</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>351</v>
+        <v>355</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>352</v>
+        <v>356</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>339</v>
+        <v>343</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -3029,42 +3059,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>355</v>
+        <v>359</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>357</v>
+        <v>361</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>359</v>
+        <v>363</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>361</v>
+        <v>365</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>363</v>
+        <v>367</v>
       </c>
     </row>
   </sheetData>
@@ -3082,18 +3112,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
   </sheetData>
@@ -3111,18 +3141,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>376</v>
+        <v>380</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
   </sheetData>
@@ -3140,18 +3170,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>376</v>
+        <v>380</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
   </sheetData>
@@ -3161,7 +3191,7 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3169,18 +3199,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>382</v>
+        <v>386</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>384</v>
+        <v>388</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>389</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>390</v>
       </c>
     </row>
   </sheetData>
@@ -3190,7 +3228,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3522,6 +3560,14 @@
       </c>
       <c r="B41" t="s" s="0">
         <v>85</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="B42" t="s" s="0">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -3539,18 +3585,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>387</v>
+        <v>393</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>389</v>
+        <v>395</v>
       </c>
     </row>
   </sheetData>
@@ -3568,250 +3614,250 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>394</v>
+        <v>400</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>395</v>
+        <v>401</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>396</v>
+        <v>402</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>398</v>
+        <v>404</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>399</v>
+        <v>405</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>400</v>
+        <v>406</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>401</v>
+        <v>407</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>402</v>
+        <v>408</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>403</v>
+        <v>409</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>405</v>
+        <v>411</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>406</v>
+        <v>412</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>407</v>
+        <v>413</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>408</v>
+        <v>414</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>410</v>
+        <v>416</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>411</v>
+        <v>417</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>412</v>
+        <v>418</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>413</v>
+        <v>419</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>414</v>
+        <v>420</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>415</v>
+        <v>421</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>416</v>
+        <v>422</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>417</v>
+        <v>423</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>418</v>
+        <v>424</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>419</v>
+        <v>425</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>420</v>
+        <v>426</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>421</v>
+        <v>427</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>422</v>
+        <v>428</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>423</v>
+        <v>429</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>424</v>
+        <v>430</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>426</v>
+        <v>432</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>427</v>
+        <v>433</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>428</v>
+        <v>434</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>429</v>
+        <v>435</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>430</v>
+        <v>436</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>431</v>
+        <v>437</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>432</v>
+        <v>438</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>433</v>
+        <v>439</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>434</v>
+        <v>440</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>435</v>
+        <v>441</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>436</v>
+        <v>442</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>438</v>
+        <v>444</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>439</v>
+        <v>445</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>440</v>
+        <v>446</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>442</v>
+        <v>448</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>444</v>
+        <v>450</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>445</v>
+        <v>451</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>446</v>
+        <v>452</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>447</v>
+        <v>453</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>448</v>
+        <v>454</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>449</v>
+        <v>455</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>450</v>
+        <v>456</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>451</v>
+        <v>457</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>452</v>
+        <v>458</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>453</v>
+        <v>459</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>454</v>
+        <v>460</v>
       </c>
     </row>
   </sheetData>
@@ -3829,138 +3875,138 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>456</v>
+        <v>462</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>457</v>
+        <v>463</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>458</v>
+        <v>464</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>459</v>
+        <v>465</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>460</v>
+        <v>466</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>461</v>
+        <v>467</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>462</v>
+        <v>468</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>463</v>
+        <v>469</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>464</v>
+        <v>470</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>465</v>
+        <v>471</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>466</v>
+        <v>472</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>467</v>
+        <v>473</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>469</v>
+        <v>475</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>470</v>
+        <v>476</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>471</v>
+        <v>477</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>442</v>
+        <v>448</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>472</v>
+        <v>478</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>473</v>
+        <v>479</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>474</v>
+        <v>480</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>475</v>
+        <v>481</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>477</v>
+        <v>483</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>478</v>
+        <v>484</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>479</v>
+        <v>485</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>480</v>
+        <v>486</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>481</v>
+        <v>487</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>482</v>
+        <v>488</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>483</v>
+        <v>489</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>484</v>
+        <v>490</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>485</v>
+        <v>491</v>
       </c>
     </row>
   </sheetData>
@@ -3978,12 +4024,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -4001,210 +4047,210 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>490</v>
+        <v>496</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>491</v>
+        <v>497</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>492</v>
+        <v>498</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>493</v>
+        <v>499</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>494</v>
+        <v>500</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>495</v>
+        <v>501</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>496</v>
+        <v>502</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>497</v>
+        <v>503</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>498</v>
+        <v>504</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>499</v>
+        <v>505</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>500</v>
+        <v>506</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>501</v>
+        <v>507</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>502</v>
+        <v>508</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>503</v>
+        <v>509</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>504</v>
+        <v>510</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>505</v>
+        <v>511</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>506</v>
+        <v>512</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>507</v>
+        <v>513</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>508</v>
+        <v>514</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>509</v>
+        <v>515</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>510</v>
+        <v>516</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>511</v>
+        <v>517</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>512</v>
+        <v>518</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>513</v>
+        <v>519</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>514</v>
+        <v>520</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>515</v>
+        <v>521</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>517</v>
+        <v>523</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>518</v>
+        <v>524</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>519</v>
+        <v>525</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>442</v>
+        <v>448</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>520</v>
+        <v>526</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>521</v>
+        <v>527</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>522</v>
+        <v>528</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>523</v>
+        <v>529</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>524</v>
+        <v>530</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>525</v>
+        <v>531</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>526</v>
+        <v>532</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>527</v>
+        <v>533</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>528</v>
+        <v>534</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>529</v>
+        <v>535</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>530</v>
+        <v>536</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>531</v>
+        <v>537</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>532</v>
+        <v>538</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>533</v>
+        <v>539</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>534</v>
+        <v>540</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>535</v>
+        <v>541</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>536</v>
+        <v>542</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>537</v>
+        <v>543</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>538</v>
+        <v>544</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>539</v>
+        <v>545</v>
       </c>
     </row>
   </sheetData>
@@ -4222,74 +4268,74 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>544</v>
+        <v>550</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>545</v>
+        <v>551</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>546</v>
+        <v>552</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>547</v>
+        <v>553</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>548</v>
+        <v>554</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>549</v>
+        <v>555</v>
       </c>
     </row>
   </sheetData>
@@ -4307,146 +4353,146 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>551</v>
+        <v>557</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>552</v>
+        <v>558</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>553</v>
+        <v>559</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>554</v>
+        <v>560</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>233</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>299</v>
+        <v>303</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>555</v>
+        <v>561</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>556</v>
+        <v>562</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>557</v>
+        <v>563</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>558</v>
+        <v>564</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>559</v>
+        <v>565</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>560</v>
+        <v>566</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>561</v>
+        <v>567</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>562</v>
+        <v>568</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>563</v>
+        <v>569</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>564</v>
+        <v>570</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>565</v>
+        <v>571</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>566</v>
+        <v>572</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>567</v>
+        <v>573</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>568</v>
+        <v>574</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>569</v>
+        <v>575</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>570</v>
+        <v>576</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>571</v>
+        <v>577</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>572</v>
+        <v>578</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>573</v>
+        <v>579</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>574</v>
+        <v>580</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>575</v>
+        <v>581</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>576</v>
+        <v>582</v>
       </c>
     </row>
   </sheetData>
@@ -4464,90 +4510,90 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>578</v>
+        <v>584</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>579</v>
+        <v>585</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>580</v>
+        <v>586</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>581</v>
+        <v>587</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>449</v>
+        <v>455</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>450</v>
+        <v>456</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>438</v>
+        <v>444</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>582</v>
+        <v>588</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>583</v>
+        <v>589</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>584</v>
+        <v>590</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>585</v>
+        <v>591</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>586</v>
+        <v>592</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>587</v>
+        <v>593</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>588</v>
+        <v>594</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>589</v>
+        <v>595</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>442</v>
+        <v>448</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>590</v>
+        <v>596</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>591</v>
+        <v>597</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>592</v>
+        <v>598</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>593</v>
+        <v>599</v>
       </c>
     </row>
   </sheetData>
@@ -4565,18 +4611,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>313</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>321</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -4586,7 +4632,7 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4594,130 +4640,146 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>597</v>
+        <v>603</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>598</v>
+        <v>604</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>599</v>
+        <v>605</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>600</v>
+        <v>606</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>601</v>
+        <v>607</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>602</v>
+        <v>608</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>603</v>
+        <v>609</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>604</v>
+        <v>610</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>605</v>
+        <v>611</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>606</v>
+        <v>612</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>607</v>
+        <v>613</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>608</v>
+        <v>614</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>442</v>
+        <v>448</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>609</v>
+        <v>615</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>610</v>
+        <v>616</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>611</v>
+        <v>617</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>612</v>
+        <v>618</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>613</v>
+        <v>619</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>614</v>
+        <v>620</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>615</v>
+        <v>621</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>616</v>
+        <v>622</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>618</v>
+        <v>624</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>619</v>
+        <v>625</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>620</v>
+        <v>626</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>621</v>
+        <v>627</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>622</v>
+        <v>628</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>623</v>
+        <v>629</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>624</v>
+        <v>630</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>625</v>
+        <v>631</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>626</v>
+        <v>632</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>633</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>635</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>636</v>
       </c>
     </row>
   </sheetData>
@@ -4735,130 +4797,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -4876,12 +4938,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -4905,30 +4967,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>630</v>
+        <v>640</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>631</v>
+        <v>641</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>633</v>
+        <v>643</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>635</v>
+        <v>645</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>632</v>
+        <v>642</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>634</v>
+        <v>644</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>636</v>
+        <v>646</v>
       </c>
     </row>
   </sheetData>
@@ -4946,12 +5008,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -4961,7 +5023,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4969,210 +5031,218 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>174</v>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>177</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -5190,546 +5260,546 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>213</v>
+        <v>217</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>219</v>
+        <v>223</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>223</v>
+        <v>227</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>225</v>
+        <v>229</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>227</v>
+        <v>231</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>231</v>
+        <v>235</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>233</v>
+        <v>237</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>235</v>
+        <v>239</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>239</v>
+        <v>243</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>241</v>
+        <v>245</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>257</v>
+        <v>261</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>267</v>
+        <v>271</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>275</v>
+        <v>279</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>279</v>
+        <v>283</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>281</v>
+        <v>285</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>283</v>
+        <v>287</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>285</v>
+        <v>289</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>287</v>
+        <v>291</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>289</v>
+        <v>293</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>291</v>
+        <v>295</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>293</v>
+        <v>297</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>295</v>
+        <v>299</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>297</v>
+        <v>301</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>299</v>
+        <v>303</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>301</v>
+        <v>305</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>303</v>
+        <v>307</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>305</v>
+        <v>309</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="0">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>307</v>
+        <v>311</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>309</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -5747,42 +5817,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>313</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>317</v>
+        <v>321</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>319</v>
+        <v>323</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>321</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -5800,26 +5870,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>317</v>
+        <v>321</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>319</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -5837,37 +5907,37 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>327</v>
+        <v>331</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>328</v>
+        <v>332</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>329</v>
+        <v>333</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>330</v>
+        <v>334</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>331</v>
+        <v>335</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>332</v>
+        <v>336</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new library preparation kits
Closes #127
</commit_message>
<xml_diff>
--- a/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
+++ b/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
@@ -448,7 +448,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="724">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -1890,6 +1890,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000342</t>
   </si>
   <si>
+    <t>10x Genomics; Chromium Next GEM Single Cell 5' HT Kit v2, 48 rxns; PN 1000356</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000467</t>
+  </si>
+  <si>
     <t>Illumina; TruSeq Stranded mRNA Library Prep (96 samples); PN 20020595</t>
   </si>
   <si>
@@ -1956,6 +1962,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000338</t>
   </si>
   <si>
+    <t>10x Genomics; Chromium Next GEM Single Cell 5' HT Kit v2, 8 rxns; PN 1000374</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000466</t>
+  </si>
+  <si>
     <t>10X Genomics; Visium CytAssist Spatial Gene Expression for FFPE, Human Transcriptome, 6.5mm, 4 reactions; PN 1000520</t>
   </si>
   <si>
@@ -2601,7 +2613,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-10-21T12:14:45-07:00</t>
+    <t>2025-10-24T14:05:47-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -2897,52 +2909,52 @@
         <v>437</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>537</v>
+        <v>541</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>538</v>
+        <v>542</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>539</v>
+        <v>543</v>
       </c>
       <c r="AO1" t="s" s="1">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="AP1" t="s" s="1">
-        <v>597</v>
+        <v>601</v>
       </c>
       <c r="AQ1" t="s" s="1">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="AR1" t="s" s="1">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="AS1" t="s" s="1">
-        <v>600</v>
+        <v>604</v>
       </c>
       <c r="AT1" t="s" s="1">
-        <v>607</v>
+        <v>611</v>
       </c>
       <c r="AU1" t="s" s="1">
-        <v>634</v>
+        <v>638</v>
       </c>
       <c r="AV1" t="s" s="1">
-        <v>653</v>
+        <v>657</v>
       </c>
       <c r="AW1" t="s" s="1">
-        <v>654</v>
+        <v>658</v>
       </c>
       <c r="AX1" t="s" s="1">
-        <v>655</v>
+        <v>659</v>
       </c>
       <c r="AY1" t="s" s="1">
-        <v>710</v>
+        <v>714</v>
       </c>
       <c r="AZ1" t="s" s="1">
-        <v>711</v>
+        <v>715</v>
       </c>
     </row>
     <row r="2">
@@ -2950,7 +2962,7 @@
         <v>98</v>
       </c>
       <c r="AZ2" t="s" s="53">
-        <v>712</v>
+        <v>716</v>
       </c>
     </row>
   </sheetData>
@@ -3053,7 +3065,7 @@
       <formula2>2147483647</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="AJ2:AJ1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'library_preparation_kit'!$A$1:$A$33</formula1>
+      <formula1>'library_preparation_kit'!$A$1:$A$35</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AK2:AK1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'sample_indexing_kit'!$A$1:$A$18</formula1>
@@ -3906,7 +3918,7 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4174,6 +4186,22 @@
       </c>
       <c r="B33" t="s" s="0">
         <v>503</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>504</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>506</v>
+      </c>
+      <c r="B35" t="s" s="0">
+        <v>507</v>
       </c>
     </row>
   </sheetData>
@@ -4191,18 +4219,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>505</v>
+        <v>509</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>506</v>
+        <v>510</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>507</v>
+        <v>511</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>508</v>
+        <v>512</v>
       </c>
     </row>
     <row r="3">
@@ -4215,122 +4243,122 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>509</v>
+        <v>513</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>510</v>
+        <v>514</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>511</v>
+        <v>515</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>512</v>
+        <v>516</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>514</v>
+        <v>518</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>515</v>
+        <v>519</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>516</v>
+        <v>520</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>517</v>
+        <v>521</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>518</v>
+        <v>522</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>520</v>
+        <v>524</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>521</v>
+        <v>525</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>522</v>
+        <v>526</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>523</v>
+        <v>527</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>524</v>
+        <v>528</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>525</v>
+        <v>529</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>526</v>
+        <v>530</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>527</v>
+        <v>531</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>528</v>
+        <v>532</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>529</v>
+        <v>533</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>530</v>
+        <v>534</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>531</v>
+        <v>535</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>532</v>
+        <v>536</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>533</v>
+        <v>537</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>534</v>
+        <v>538</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>535</v>
+        <v>539</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>536</v>
+        <v>540</v>
       </c>
     </row>
   </sheetData>
@@ -4371,234 +4399,234 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>541</v>
+        <v>545</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>542</v>
+        <v>546</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>543</v>
+        <v>547</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>544</v>
+        <v>548</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>546</v>
+        <v>550</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>547</v>
+        <v>551</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>548</v>
+        <v>552</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>549</v>
+        <v>553</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>550</v>
+        <v>554</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>551</v>
+        <v>555</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>552</v>
+        <v>556</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>553</v>
+        <v>557</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>554</v>
+        <v>558</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>555</v>
+        <v>559</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>556</v>
+        <v>560</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>557</v>
+        <v>561</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>558</v>
+        <v>562</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>559</v>
+        <v>563</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>560</v>
+        <v>564</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>562</v>
+        <v>566</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>563</v>
+        <v>567</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>564</v>
+        <v>568</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>566</v>
+        <v>570</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>567</v>
+        <v>571</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>568</v>
+        <v>572</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>569</v>
+        <v>573</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>570</v>
+        <v>574</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>571</v>
+        <v>575</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>572</v>
+        <v>576</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>573</v>
+        <v>577</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>574</v>
+        <v>578</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>575</v>
+        <v>579</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>576</v>
+        <v>580</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>577</v>
+        <v>581</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>578</v>
+        <v>582</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>579</v>
+        <v>583</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>580</v>
+        <v>584</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>581</v>
+        <v>585</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>582</v>
+        <v>586</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>583</v>
+        <v>587</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>584</v>
+        <v>588</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>585</v>
+        <v>589</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>586</v>
+        <v>590</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>587</v>
+        <v>591</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>588</v>
+        <v>592</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>589</v>
+        <v>593</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>590</v>
+        <v>594</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>591</v>
+        <v>595</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>592</v>
+        <v>596</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>593</v>
+        <v>597</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>594</v>
+        <v>598</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>595</v>
+        <v>599</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>596</v>
+        <v>600</v>
       </c>
     </row>
   </sheetData>
@@ -4648,18 +4676,18 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>601</v>
+        <v>605</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>602</v>
+        <v>606</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>603</v>
+        <v>607</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>604</v>
+        <v>608</v>
       </c>
     </row>
     <row r="7">
@@ -4680,10 +4708,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>605</v>
+        <v>609</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>606</v>
+        <v>610</v>
       </c>
     </row>
   </sheetData>
@@ -4717,10 +4745,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>608</v>
+        <v>612</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>609</v>
+        <v>613</v>
       </c>
     </row>
     <row r="4">
@@ -4733,10 +4761,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>610</v>
+        <v>614</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>611</v>
+        <v>615</v>
       </c>
     </row>
     <row r="6">
@@ -4757,90 +4785,90 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>612</v>
+        <v>616</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>613</v>
+        <v>617</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>614</v>
+        <v>618</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>615</v>
+        <v>619</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>617</v>
+        <v>621</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>618</v>
+        <v>622</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>619</v>
+        <v>623</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>620</v>
+        <v>624</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>621</v>
+        <v>625</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>622</v>
+        <v>626</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>623</v>
+        <v>627</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>624</v>
+        <v>628</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>625</v>
+        <v>629</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>626</v>
+        <v>630</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>627</v>
+        <v>631</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>628</v>
+        <v>632</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>629</v>
+        <v>633</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>630</v>
+        <v>634</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>631</v>
+        <v>635</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>632</v>
+        <v>636</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>633</v>
+        <v>637</v>
       </c>
     </row>
   </sheetData>
@@ -4858,98 +4886,98 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>635</v>
+        <v>639</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>636</v>
+        <v>640</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>637</v>
+        <v>641</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>638</v>
+        <v>642</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>499</v>
+        <v>501</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>639</v>
+        <v>643</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>640</v>
+        <v>644</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>485</v>
+        <v>487</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>641</v>
+        <v>645</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>642</v>
+        <v>646</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>643</v>
+        <v>647</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>644</v>
+        <v>648</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>645</v>
+        <v>649</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>646</v>
+        <v>650</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>647</v>
+        <v>651</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>648</v>
+        <v>652</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>649</v>
+        <v>653</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>650</v>
+        <v>654</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>651</v>
+        <v>655</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>652</v>
+        <v>656</v>
       </c>
     </row>
   </sheetData>
@@ -4996,226 +5024,226 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>656</v>
+        <v>660</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>657</v>
+        <v>661</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>658</v>
+        <v>662</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>659</v>
+        <v>663</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>660</v>
+        <v>664</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>661</v>
+        <v>665</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>662</v>
+        <v>666</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>663</v>
+        <v>667</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>664</v>
+        <v>668</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>665</v>
+        <v>669</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>666</v>
+        <v>670</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>667</v>
+        <v>671</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>668</v>
+        <v>672</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>669</v>
+        <v>673</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>670</v>
+        <v>674</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>671</v>
+        <v>675</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>672</v>
+        <v>676</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>673</v>
+        <v>677</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>674</v>
+        <v>678</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>675</v>
+        <v>679</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>676</v>
+        <v>680</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>677</v>
+        <v>681</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>678</v>
+        <v>682</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>679</v>
+        <v>683</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>680</v>
+        <v>684</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>681</v>
+        <v>685</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>682</v>
+        <v>686</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>683</v>
+        <v>687</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>684</v>
+        <v>688</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>685</v>
+        <v>689</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>686</v>
+        <v>690</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>687</v>
+        <v>691</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>688</v>
+        <v>692</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>689</v>
+        <v>693</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>690</v>
+        <v>694</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>691</v>
+        <v>695</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>692</v>
+        <v>696</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>693</v>
+        <v>697</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>694</v>
+        <v>698</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>695</v>
+        <v>699</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>696</v>
+        <v>700</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>697</v>
+        <v>701</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>698</v>
+        <v>702</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>699</v>
+        <v>703</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>700</v>
+        <v>704</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>701</v>
+        <v>705</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>702</v>
+        <v>706</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>703</v>
+        <v>707</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>704</v>
+        <v>708</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>705</v>
+        <v>709</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>706</v>
+        <v>710</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>707</v>
+        <v>711</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>708</v>
+        <v>712</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>709</v>
+        <v>713</v>
       </c>
     </row>
   </sheetData>
@@ -5403,16 +5431,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>713</v>
+        <v>717</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>714</v>
+        <v>718</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>716</v>
+        <v>720</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>718</v>
+        <v>722</v>
       </c>
     </row>
     <row r="2">
@@ -5420,13 +5448,13 @@
         <v>98</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>715</v>
+        <v>719</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>717</v>
+        <v>721</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>719</v>
+        <v>723</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new oligo panel
Closes #144
</commit_message>
<xml_diff>
--- a/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
+++ b/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
@@ -448,7 +448,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="742">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="770">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -552,6 +552,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
   </si>
   <si>
+    <t>iCLAP</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000479</t>
+  </si>
+  <si>
     <t>seqFISH</t>
   </si>
   <si>
@@ -618,6 +624,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000207</t>
   </si>
   <si>
+    <t>MACSima</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000480</t>
+  </si>
+  <si>
     <t>CyTOF</t>
   </si>
   <si>
@@ -801,6 +813,12 @@
     <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C13201</t>
   </si>
   <si>
+    <t>Lipid + metabolite + protein</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000478</t>
+  </si>
+  <si>
     <t>RNA + protein</t>
   </si>
   <si>
@@ -987,6 +1005,12 @@
     <t>https://identifiers.org/RRID:SCR_023605</t>
   </si>
   <si>
+    <t>Waters</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024589</t>
+  </si>
+  <si>
     <t>In-House</t>
   </si>
   <si>
@@ -1041,12 +1065,24 @@
     <t>https://identifiers.org/RRID:SCR_023604</t>
   </si>
   <si>
+    <t>Miltenyi Biotec</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_008984</t>
+  </si>
+  <si>
     <t>Leica Biosystems</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_023603</t>
   </si>
   <si>
+    <t>Revvity</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027779</t>
+  </si>
+  <si>
     <t>Cytek Biosciences</t>
   </si>
   <si>
@@ -1176,6 +1212,18 @@
     <t>https://identifiers.org/RRID:SCR_026452</t>
   </si>
   <si>
+    <t>DMi8</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026672</t>
+  </si>
+  <si>
+    <t>Opera Phenix Plus HCS</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027780</t>
+  </si>
+  <si>
     <t>timsTOF Pro 2</t>
   </si>
   <si>
@@ -1218,6 +1266,12 @@
     <t>https://identifiers.org/RRID:SCR_027101</t>
   </si>
   <si>
+    <t>Orbitrap Fusion Tribrid</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020559</t>
+  </si>
+  <si>
     <t>Custom: Multiphoton</t>
   </si>
   <si>
@@ -1344,6 +1398,18 @@
     <t>https://identifiers.org/RRID:SCR_027072</t>
   </si>
   <si>
+    <t>Opera Phenix HCS</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027817</t>
+  </si>
+  <si>
+    <t>Zeiss LightSheet Z.1</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020919</t>
+  </si>
+  <si>
     <t>IN Cell Analyzer 2200</t>
   </si>
   <si>
@@ -1485,6 +1551,18 @@
     <t>https://identifiers.org/RRID:SCR_023613</t>
   </si>
   <si>
+    <t>SYNAPT G2-Si</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027782</t>
+  </si>
+  <si>
+    <t>MACSima System</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027923</t>
+  </si>
+  <si>
     <t>Biomark HD</t>
   </si>
   <si>
@@ -2502,6 +2580,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000442</t>
   </si>
   <si>
+    <t>10x Genomics; GEM-X Flex Human Transcriptome Probe Kit, 16 samples; PN 1000785</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000481</t>
+  </si>
+  <si>
     <t>10x Genomics; Visium Human Transcriptome Probe Kit-Small; PN 1000363</t>
   </si>
   <si>
@@ -2667,7 +2751,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-12-08T11:16:37-08:00</t>
+    <t>2026-02-11T13:56:48-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -2867,174 +2951,174 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>209</v>
+        <v>221</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>361</v>
+        <v>387</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>362</v>
+        <v>388</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>373</v>
+        <v>399</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>374</v>
+        <v>400</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>375</v>
+        <v>401</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>376</v>
+        <v>402</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>377</v>
+        <v>403</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>386</v>
+        <v>412</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>391</v>
+        <v>417</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>397</v>
+        <v>423</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>399</v>
+        <v>425</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>400</v>
+        <v>426</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>404</v>
+        <v>430</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>415</v>
+        <v>441</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>416</v>
+        <v>442</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>417</v>
+        <v>443</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>422</v>
+        <v>448</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>423</v>
+        <v>449</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>424</v>
+        <v>450</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>425</v>
+        <v>451</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>428</v>
+        <v>454</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>429</v>
+        <v>455</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>430</v>
+        <v>456</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>431</v>
+        <v>457</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>438</v>
+        <v>464</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>443</v>
+        <v>469</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>444</v>
+        <v>470</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>445</v>
+        <v>471</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>520</v>
+        <v>546</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>555</v>
+        <v>581</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>556</v>
+        <v>582</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>557</v>
+        <v>583</v>
       </c>
       <c r="AO1" t="s" s="1">
-        <v>558</v>
+        <v>584</v>
       </c>
       <c r="AP1" t="s" s="1">
-        <v>615</v>
+        <v>641</v>
       </c>
       <c r="AQ1" t="s" s="1">
-        <v>616</v>
+        <v>642</v>
       </c>
       <c r="AR1" t="s" s="1">
-        <v>617</v>
+        <v>643</v>
       </c>
       <c r="AS1" t="s" s="1">
-        <v>618</v>
+        <v>644</v>
       </c>
       <c r="AT1" t="s" s="1">
-        <v>625</v>
+        <v>651</v>
       </c>
       <c r="AU1" t="s" s="1">
-        <v>652</v>
+        <v>678</v>
       </c>
       <c r="AV1" t="s" s="1">
-        <v>673</v>
+        <v>699</v>
       </c>
       <c r="AW1" t="s" s="1">
-        <v>674</v>
+        <v>700</v>
       </c>
       <c r="AX1" t="s" s="1">
-        <v>675</v>
+        <v>701</v>
       </c>
       <c r="AY1" t="s" s="1">
-        <v>732</v>
+        <v>760</v>
       </c>
       <c r="AZ1" t="s" s="1">
-        <v>733</v>
+        <v>761</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="AZ2" t="s" s="53">
-        <v>734</v>
+        <v>762</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="41">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$53</formula1>
+      <formula1>'dataset_type'!$A$1:$A$55</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'analyte_class'!$A$1:$A$17</formula1>
+      <formula1>'analyte_class'!$A$1:$A$18</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="F2:F1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$30</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$33</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$77</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$84</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -3151,7 +3235,7 @@
       <formula1>'probe_hybridization_time_unit'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AX2:AX1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'oligo_probe_panel'!$A$1:$A$29</formula1>
+      <formula1>'oligo_probe_panel'!$A$1:$A$30</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AY2:AY1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_custom_probes_used'!$A$1:$A$2</formula1>
@@ -3173,26 +3257,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>387</v>
+        <v>413</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>388</v>
+        <v>414</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>219</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>389</v>
+        <v>415</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>390</v>
+        <v>416</v>
       </c>
     </row>
   </sheetData>
@@ -3210,32 +3294,32 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>392</v>
+        <v>418</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>393</v>
+        <v>419</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>394</v>
+        <v>420</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>395</v>
+        <v>421</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>396</v>
+        <v>422</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>218</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -3253,22 +3337,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>378</v>
+        <v>404</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>393</v>
+        <v>419</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>398</v>
+        <v>424</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>218</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -3286,26 +3370,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>387</v>
+        <v>413</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>388</v>
+        <v>414</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>219</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>389</v>
+        <v>415</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>390</v>
+        <v>416</v>
       </c>
     </row>
   </sheetData>
@@ -3323,27 +3407,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>379</v>
+        <v>405</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>401</v>
+        <v>427</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>402</v>
+        <v>428</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>403</v>
+        <v>429</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>218</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -3361,42 +3445,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>405</v>
+        <v>431</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>406</v>
+        <v>432</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>407</v>
+        <v>433</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>408</v>
+        <v>434</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>409</v>
+        <v>435</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>410</v>
+        <v>436</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>411</v>
+        <v>437</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>412</v>
+        <v>438</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>413</v>
+        <v>439</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>414</v>
+        <v>440</v>
       </c>
     </row>
   </sheetData>
@@ -3414,18 +3498,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>418</v>
+        <v>444</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>419</v>
+        <v>445</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>420</v>
+        <v>446</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>421</v>
+        <v>447</v>
       </c>
     </row>
   </sheetData>
@@ -3443,18 +3527,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>426</v>
+        <v>452</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>427</v>
+        <v>453</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>420</v>
+        <v>446</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>421</v>
+        <v>447</v>
       </c>
     </row>
   </sheetData>
@@ -3472,18 +3556,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>426</v>
+        <v>452</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>427</v>
+        <v>453</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>420</v>
+        <v>446</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>421</v>
+        <v>447</v>
       </c>
     </row>
   </sheetData>
@@ -3501,26 +3585,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>432</v>
+        <v>458</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>433</v>
+        <v>459</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>434</v>
+        <v>460</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>435</v>
+        <v>461</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>436</v>
+        <v>462</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>437</v>
+        <v>463</v>
       </c>
     </row>
   </sheetData>
@@ -3530,7 +3614,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3958,6 +4042,22 @@
       </c>
       <c r="B53" t="s" s="0">
         <v>109</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="0">
+        <v>110</v>
+      </c>
+      <c r="B54" t="s" s="0">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="0">
+        <v>112</v>
+      </c>
+      <c r="B55" t="s" s="0">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -3975,18 +4075,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>439</v>
+        <v>465</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>440</v>
+        <v>466</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>441</v>
+        <v>467</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>442</v>
+        <v>468</v>
       </c>
     </row>
   </sheetData>
@@ -4004,298 +4104,298 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>446</v>
+        <v>472</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>447</v>
+        <v>473</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>448</v>
+        <v>474</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>449</v>
+        <v>475</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>450</v>
+        <v>476</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>451</v>
+        <v>477</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>452</v>
+        <v>478</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>453</v>
+        <v>479</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>454</v>
+        <v>480</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>455</v>
+        <v>481</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>456</v>
+        <v>482</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>457</v>
+        <v>483</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>458</v>
+        <v>484</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>459</v>
+        <v>485</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>460</v>
+        <v>486</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>461</v>
+        <v>487</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>462</v>
+        <v>488</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>463</v>
+        <v>489</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>464</v>
+        <v>490</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>465</v>
+        <v>491</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>466</v>
+        <v>492</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>467</v>
+        <v>493</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>468</v>
+        <v>494</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>469</v>
+        <v>495</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>470</v>
+        <v>496</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>471</v>
+        <v>497</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>472</v>
+        <v>498</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>473</v>
+        <v>499</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>474</v>
+        <v>500</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>475</v>
+        <v>501</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>476</v>
+        <v>502</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>477</v>
+        <v>503</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>478</v>
+        <v>504</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>479</v>
+        <v>505</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>480</v>
+        <v>506</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>481</v>
+        <v>507</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>482</v>
+        <v>508</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>483</v>
+        <v>509</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>484</v>
+        <v>510</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>485</v>
+        <v>511</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>486</v>
+        <v>512</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>487</v>
+        <v>513</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>488</v>
+        <v>514</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>489</v>
+        <v>515</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>490</v>
+        <v>516</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>491</v>
+        <v>517</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>492</v>
+        <v>518</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>493</v>
+        <v>519</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>494</v>
+        <v>520</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>495</v>
+        <v>521</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>496</v>
+        <v>522</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>497</v>
+        <v>523</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>498</v>
+        <v>524</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>499</v>
+        <v>525</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>500</v>
+        <v>526</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>501</v>
+        <v>527</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>502</v>
+        <v>528</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>503</v>
+        <v>529</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>504</v>
+        <v>530</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>505</v>
+        <v>531</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>506</v>
+        <v>532</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>507</v>
+        <v>533</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>508</v>
+        <v>534</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>509</v>
+        <v>535</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>510</v>
+        <v>536</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>511</v>
+        <v>537</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>512</v>
+        <v>538</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>513</v>
+        <v>539</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>514</v>
+        <v>540</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>515</v>
+        <v>541</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>516</v>
+        <v>542</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>517</v>
+        <v>543</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>518</v>
+        <v>544</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>519</v>
+        <v>545</v>
       </c>
     </row>
   </sheetData>
@@ -4313,154 +4413,154 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>521</v>
+        <v>547</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>522</v>
+        <v>548</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>523</v>
+        <v>549</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>524</v>
+        <v>550</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>219</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>525</v>
+        <v>551</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>526</v>
+        <v>552</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>527</v>
+        <v>553</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>528</v>
+        <v>554</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>529</v>
+        <v>555</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>530</v>
+        <v>556</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>531</v>
+        <v>557</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>532</v>
+        <v>558</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>533</v>
+        <v>559</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>534</v>
+        <v>560</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>535</v>
+        <v>561</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>536</v>
+        <v>562</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>537</v>
+        <v>563</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>538</v>
+        <v>564</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>502</v>
+        <v>528</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>503</v>
+        <v>529</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>539</v>
+        <v>565</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>540</v>
+        <v>566</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>541</v>
+        <v>567</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>542</v>
+        <v>568</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>543</v>
+        <v>569</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>544</v>
+        <v>570</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>545</v>
+        <v>571</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>546</v>
+        <v>572</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>547</v>
+        <v>573</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>548</v>
+        <v>574</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>549</v>
+        <v>575</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>550</v>
+        <v>576</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>551</v>
+        <v>577</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>552</v>
+        <v>578</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>553</v>
+        <v>579</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>554</v>
+        <v>580</v>
       </c>
     </row>
   </sheetData>
@@ -4478,12 +4578,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -4501,234 +4601,234 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>559</v>
+        <v>585</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>560</v>
+        <v>586</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>561</v>
+        <v>587</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>562</v>
+        <v>588</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>563</v>
+        <v>589</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>564</v>
+        <v>590</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>565</v>
+        <v>591</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>566</v>
+        <v>592</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>567</v>
+        <v>593</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>568</v>
+        <v>594</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>569</v>
+        <v>595</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>570</v>
+        <v>596</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>571</v>
+        <v>597</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>572</v>
+        <v>598</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>573</v>
+        <v>599</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>574</v>
+        <v>600</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>575</v>
+        <v>601</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>576</v>
+        <v>602</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>577</v>
+        <v>603</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>578</v>
+        <v>604</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>579</v>
+        <v>605</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>580</v>
+        <v>606</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>581</v>
+        <v>607</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>582</v>
+        <v>608</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>583</v>
+        <v>609</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>584</v>
+        <v>610</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>585</v>
+        <v>611</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>586</v>
+        <v>612</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>587</v>
+        <v>613</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>588</v>
+        <v>614</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>589</v>
+        <v>615</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>590</v>
+        <v>616</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>591</v>
+        <v>617</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>592</v>
+        <v>618</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>502</v>
+        <v>528</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>503</v>
+        <v>529</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>593</v>
+        <v>619</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>594</v>
+        <v>620</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>595</v>
+        <v>621</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>596</v>
+        <v>622</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>597</v>
+        <v>623</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>598</v>
+        <v>624</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>599</v>
+        <v>625</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>600</v>
+        <v>626</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>601</v>
+        <v>627</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>602</v>
+        <v>628</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>603</v>
+        <v>629</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>604</v>
+        <v>630</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>605</v>
+        <v>631</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>606</v>
+        <v>632</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>607</v>
+        <v>633</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>608</v>
+        <v>634</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>609</v>
+        <v>635</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>610</v>
+        <v>636</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>611</v>
+        <v>637</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>612</v>
+        <v>638</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>613</v>
+        <v>639</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>614</v>
+        <v>640</v>
       </c>
     </row>
   </sheetData>
@@ -4746,90 +4846,90 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>180</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>198</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>219</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>619</v>
+        <v>645</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>620</v>
+        <v>646</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>621</v>
+        <v>647</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>622</v>
+        <v>648</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>201</v>
+        <v>213</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>202</v>
+        <v>214</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>206</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>166</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>623</v>
+        <v>649</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>624</v>
+        <v>650</v>
       </c>
     </row>
   </sheetData>
@@ -4847,154 +4947,154 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>290</v>
+        <v>308</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>291</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>219</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>626</v>
+        <v>652</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>627</v>
+        <v>653</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>223</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>628</v>
+        <v>654</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>629</v>
+        <v>655</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>502</v>
+        <v>528</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>503</v>
+        <v>529</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>270</v>
+        <v>288</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>271</v>
+        <v>289</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>347</v>
+        <v>373</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>348</v>
+        <v>374</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>630</v>
+        <v>656</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>631</v>
+        <v>657</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>632</v>
+        <v>658</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>633</v>
+        <v>659</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>634</v>
+        <v>660</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>635</v>
+        <v>661</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>636</v>
+        <v>662</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>637</v>
+        <v>663</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>638</v>
+        <v>664</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>639</v>
+        <v>665</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>640</v>
+        <v>666</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>641</v>
+        <v>667</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>642</v>
+        <v>668</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>643</v>
+        <v>669</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>644</v>
+        <v>670</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>645</v>
+        <v>671</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>646</v>
+        <v>672</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>647</v>
+        <v>673</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>648</v>
+        <v>674</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>649</v>
+        <v>675</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>650</v>
+        <v>676</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>651</v>
+        <v>677</v>
       </c>
     </row>
   </sheetData>
@@ -5012,106 +5112,106 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>653</v>
+        <v>679</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>654</v>
+        <v>680</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>655</v>
+        <v>681</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>656</v>
+        <v>682</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>498</v>
+        <v>524</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>499</v>
+        <v>525</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>657</v>
+        <v>683</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>658</v>
+        <v>684</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>659</v>
+        <v>685</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>660</v>
+        <v>686</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>661</v>
+        <v>687</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>662</v>
+        <v>688</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>502</v>
+        <v>528</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>503</v>
+        <v>529</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>663</v>
+        <v>689</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>664</v>
+        <v>690</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>665</v>
+        <v>691</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>666</v>
+        <v>692</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>512</v>
+        <v>538</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>513</v>
+        <v>539</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>667</v>
+        <v>693</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>668</v>
+        <v>694</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>669</v>
+        <v>695</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>670</v>
+        <v>696</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>671</v>
+        <v>697</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>672</v>
+        <v>698</v>
       </c>
     </row>
   </sheetData>
@@ -5129,18 +5229,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>363</v>
+        <v>389</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>364</v>
+        <v>390</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>371</v>
+        <v>397</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>372</v>
+        <v>398</v>
       </c>
     </row>
   </sheetData>
@@ -5150,7 +5250,7 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5158,234 +5258,242 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>676</v>
+        <v>702</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>677</v>
+        <v>703</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>678</v>
+        <v>704</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>679</v>
+        <v>705</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>680</v>
+        <v>706</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>681</v>
+        <v>707</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>682</v>
+        <v>708</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>683</v>
+        <v>709</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>684</v>
+        <v>710</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>685</v>
+        <v>711</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>686</v>
+        <v>712</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>687</v>
+        <v>713</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>688</v>
+        <v>714</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>689</v>
+        <v>715</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>690</v>
+        <v>716</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>691</v>
+        <v>717</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>692</v>
+        <v>718</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>693</v>
+        <v>719</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>694</v>
+        <v>720</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>695</v>
+        <v>721</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>696</v>
+        <v>722</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>697</v>
+        <v>723</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>698</v>
+        <v>724</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>699</v>
+        <v>725</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>700</v>
+        <v>726</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>701</v>
+        <v>727</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>702</v>
+        <v>728</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>703</v>
+        <v>729</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>704</v>
+        <v>730</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>705</v>
+        <v>731</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>706</v>
+        <v>732</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>707</v>
+        <v>733</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>708</v>
+        <v>734</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>709</v>
+        <v>735</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>710</v>
+        <v>736</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>711</v>
+        <v>737</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>712</v>
+        <v>738</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>713</v>
+        <v>739</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>714</v>
+        <v>740</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>715</v>
+        <v>741</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>716</v>
+        <v>742</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>717</v>
+        <v>743</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>502</v>
+        <v>744</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>503</v>
+        <v>745</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>718</v>
+        <v>528</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>719</v>
+        <v>529</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>720</v>
+        <v>746</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>721</v>
+        <v>747</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>722</v>
+        <v>748</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>723</v>
+        <v>749</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>724</v>
+        <v>750</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>725</v>
+        <v>751</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>726</v>
+        <v>752</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>727</v>
+        <v>753</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>728</v>
+        <v>754</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>729</v>
+        <v>755</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>730</v>
+        <v>756</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>731</v>
+        <v>757</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>758</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>759</v>
       </c>
     </row>
   </sheetData>
@@ -5395,7 +5503,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5403,138 +5511,146 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>144</v>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>149</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -5552,12 +5668,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -5581,30 +5697,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>735</v>
+        <v>763</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>736</v>
+        <v>764</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>738</v>
+        <v>766</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>740</v>
+        <v>768</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>737</v>
+        <v>765</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>739</v>
+        <v>767</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>741</v>
+        <v>769</v>
       </c>
     </row>
   </sheetData>
@@ -5622,12 +5738,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -5637,7 +5753,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5645,242 +5761,266 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>150</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>152</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>158</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>160</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>164</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>166</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>168</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>170</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>174</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>186</v>
+        <v>192</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>188</v>
+        <v>194</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>190</v>
+        <v>196</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>192</v>
+        <v>198</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>194</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>196</v>
+        <v>202</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>198</v>
+        <v>204</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>200</v>
+        <v>206</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>202</v>
+        <v>208</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>204</v>
+        <v>210</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>206</v>
+        <v>212</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>208</v>
+        <v>214</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>215</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>217</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>219</v>
+      </c>
+      <c r="B33" t="s" s="0">
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -5890,7 +6030,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B77"/>
+  <dimension ref="A1:B84"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5898,618 +6038,674 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>210</v>
+        <v>222</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>211</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>212</v>
+        <v>224</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>213</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>215</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>216</v>
+        <v>228</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>217</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>219</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>220</v>
+        <v>232</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>221</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>223</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>224</v>
+        <v>236</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>225</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>226</v>
+        <v>238</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>227</v>
+        <v>239</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>228</v>
+        <v>240</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>229</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>230</v>
+        <v>242</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>231</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>233</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>234</v>
+        <v>246</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>235</v>
+        <v>247</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>237</v>
+        <v>249</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>238</v>
+        <v>250</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>239</v>
+        <v>251</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>240</v>
+        <v>252</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>241</v>
+        <v>253</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>242</v>
+        <v>254</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>243</v>
+        <v>255</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>245</v>
+        <v>257</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>246</v>
+        <v>258</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>247</v>
+        <v>259</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>248</v>
+        <v>260</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>249</v>
+        <v>261</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>250</v>
+        <v>262</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>251</v>
+        <v>263</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>253</v>
+        <v>265</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>255</v>
+        <v>267</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>256</v>
+        <v>268</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>257</v>
+        <v>269</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>258</v>
+        <v>270</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>259</v>
+        <v>271</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>260</v>
+        <v>272</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>261</v>
+        <v>273</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>262</v>
+        <v>274</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>263</v>
+        <v>275</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>264</v>
+        <v>276</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>265</v>
+        <v>277</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>266</v>
+        <v>278</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>267</v>
+        <v>279</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>268</v>
+        <v>280</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>269</v>
+        <v>281</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>270</v>
+        <v>282</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>271</v>
+        <v>283</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>273</v>
+        <v>285</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>274</v>
+        <v>286</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>275</v>
+        <v>287</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>277</v>
+        <v>289</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>278</v>
+        <v>290</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>279</v>
+        <v>291</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>280</v>
+        <v>292</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>281</v>
+        <v>293</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>282</v>
+        <v>294</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>283</v>
+        <v>295</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>284</v>
+        <v>296</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>285</v>
+        <v>297</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>286</v>
+        <v>298</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>287</v>
+        <v>299</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>289</v>
+        <v>301</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>290</v>
+        <v>302</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>291</v>
+        <v>303</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>292</v>
+        <v>304</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>293</v>
+        <v>305</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>294</v>
+        <v>306</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>295</v>
+        <v>307</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>296</v>
+        <v>308</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>297</v>
+        <v>309</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>298</v>
+        <v>310</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>300</v>
+        <v>312</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>301</v>
+        <v>313</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>302</v>
+        <v>314</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>303</v>
+        <v>315</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>304</v>
+        <v>316</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>305</v>
+        <v>317</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>306</v>
+        <v>318</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>307</v>
+        <v>319</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>308</v>
+        <v>320</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>309</v>
+        <v>321</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>310</v>
+        <v>322</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>311</v>
+        <v>323</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>312</v>
+        <v>324</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>313</v>
+        <v>325</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>314</v>
+        <v>326</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>315</v>
+        <v>327</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>316</v>
+        <v>328</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>317</v>
+        <v>329</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>318</v>
+        <v>330</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>319</v>
+        <v>331</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>320</v>
+        <v>332</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>321</v>
+        <v>333</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>322</v>
+        <v>334</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>323</v>
+        <v>335</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>324</v>
+        <v>336</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>325</v>
+        <v>337</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>326</v>
+        <v>338</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>327</v>
+        <v>339</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>70</v>
+        <v>340</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>328</v>
+        <v>341</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>329</v>
+        <v>342</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>330</v>
+        <v>343</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>331</v>
+        <v>344</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>332</v>
+        <v>345</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>333</v>
+        <v>346</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>334</v>
+        <v>347</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>179</v>
+        <v>348</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>180</v>
+        <v>349</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>335</v>
+        <v>74</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>336</v>
+        <v>350</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>338</v>
+        <v>352</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="0">
-        <v>339</v>
+        <v>353</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>340</v>
+        <v>354</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>341</v>
+        <v>355</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>342</v>
+        <v>356</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s" s="0">
-        <v>343</v>
+        <v>187</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>344</v>
+        <v>188</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s" s="0">
-        <v>345</v>
+        <v>357</v>
       </c>
       <c r="B70" t="s" s="0">
-        <v>346</v>
+        <v>358</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s" s="0">
-        <v>347</v>
+        <v>359</v>
       </c>
       <c r="B71" t="s" s="0">
-        <v>348</v>
+        <v>360</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s" s="0">
-        <v>349</v>
+        <v>361</v>
       </c>
       <c r="B72" t="s" s="0">
-        <v>350</v>
+        <v>362</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s" s="0">
-        <v>351</v>
+        <v>363</v>
       </c>
       <c r="B73" t="s" s="0">
-        <v>352</v>
+        <v>364</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s" s="0">
-        <v>353</v>
+        <v>365</v>
       </c>
       <c r="B74" t="s" s="0">
-        <v>354</v>
+        <v>366</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s" s="0">
-        <v>355</v>
+        <v>367</v>
       </c>
       <c r="B75" t="s" s="0">
-        <v>356</v>
+        <v>368</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s" s="0">
-        <v>357</v>
+        <v>369</v>
       </c>
       <c r="B76" t="s" s="0">
-        <v>358</v>
+        <v>370</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s" s="0">
-        <v>359</v>
+        <v>371</v>
       </c>
       <c r="B77" t="s" s="0">
-        <v>360</v>
+        <v>372</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s" s="0">
+        <v>373</v>
+      </c>
+      <c r="B78" t="s" s="0">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s" s="0">
+        <v>375</v>
+      </c>
+      <c r="B79" t="s" s="0">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s" s="0">
+        <v>377</v>
+      </c>
+      <c r="B80" t="s" s="0">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s" s="0">
+        <v>379</v>
+      </c>
+      <c r="B81" t="s" s="0">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s" s="0">
+        <v>381</v>
+      </c>
+      <c r="B82" t="s" s="0">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s" s="0">
+        <v>383</v>
+      </c>
+      <c r="B83" t="s" s="0">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s" s="0">
+        <v>385</v>
+      </c>
+      <c r="B84" t="s" s="0">
+        <v>386</v>
       </c>
     </row>
   </sheetData>
@@ -6527,42 +6723,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>363</v>
+        <v>389</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>364</v>
+        <v>390</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>365</v>
+        <v>391</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>366</v>
+        <v>392</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>367</v>
+        <v>393</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>368</v>
+        <v>394</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>369</v>
+        <v>395</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>370</v>
+        <v>396</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>371</v>
+        <v>397</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>372</v>
+        <v>398</v>
       </c>
     </row>
   </sheetData>
@@ -6580,26 +6776,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>365</v>
+        <v>391</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>366</v>
+        <v>392</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>367</v>
+        <v>393</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>368</v>
+        <v>394</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>369</v>
+        <v>395</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>370</v>
+        <v>396</v>
       </c>
     </row>
   </sheetData>
@@ -6617,47 +6813,47 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>378</v>
+        <v>404</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>379</v>
+        <v>405</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>380</v>
+        <v>406</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>381</v>
+        <v>407</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>382</v>
+        <v>408</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>383</v>
+        <v>409</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>384</v>
+        <v>410</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>385</v>
+        <v>411</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>218</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 14 as a new UMI size
Closes #146
</commit_message>
<xml_diff>
--- a/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
+++ b/rnaseq-with-probes/latest/rnaseq-with-probes.xlsx
@@ -448,7 +448,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="770">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="772">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -1482,6 +1482,12 @@
     <t>https://identifiers.org/RRID:SCR_023692</t>
   </si>
   <si>
+    <t>NanoZoomer 2.0-RS</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_028001</t>
+  </si>
+  <si>
     <t>Axio Observer 3</t>
   </si>
   <si>
@@ -2751,7 +2757,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2026-02-11T13:56:48-08:00</t>
+    <t>2026-02-23T13:18:56-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -2963,136 +2969,136 @@
         <v>221</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="AO1" t="s" s="1">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="AP1" t="s" s="1">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="AQ1" t="s" s="1">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="AR1" t="s" s="1">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="AS1" t="s" s="1">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="AT1" t="s" s="1">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="AU1" t="s" s="1">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="AV1" t="s" s="1">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="AW1" t="s" s="1">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="AX1" t="s" s="1">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="AY1" t="s" s="1">
-        <v>760</v>
+        <v>762</v>
       </c>
       <c r="AZ1" t="s" s="1">
-        <v>761</v>
+        <v>763</v>
       </c>
     </row>
     <row r="2">
@@ -3100,7 +3106,7 @@
         <v>106</v>
       </c>
       <c r="AZ2" t="s" s="53">
-        <v>762</v>
+        <v>764</v>
       </c>
     </row>
   </sheetData>
@@ -3118,7 +3124,7 @@
       <formula1>'acquisition_instrument_vendor'!$A$1:$A$33</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$84</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$85</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -3150,7 +3156,7 @@
       <formula1>'umi_read'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="T2:T1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'umi_size'!$A$1:$A$5</formula1>
+      <formula1>'umi_size'!$A$1:$A$6</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="U2:U1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'assay_input_entity'!$A$1:$A$5</formula1>
@@ -3257,10 +3263,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>414</v>
+        <v>416</v>
       </c>
     </row>
     <row r="2">
@@ -3273,10 +3279,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>416</v>
+        <v>418</v>
       </c>
     </row>
   </sheetData>
@@ -3294,27 +3300,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>418</v>
+        <v>420</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>419</v>
+        <v>421</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>420</v>
+        <v>422</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>421</v>
+        <v>423</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>422</v>
+        <v>424</v>
       </c>
     </row>
     <row r="6">
@@ -3337,17 +3343,17 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>404</v>
+        <v>406</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>419</v>
+        <v>421</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>424</v>
+        <v>426</v>
       </c>
     </row>
     <row r="4">
@@ -3370,10 +3376,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>414</v>
+        <v>416</v>
       </c>
     </row>
     <row r="2">
@@ -3386,10 +3392,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>416</v>
+        <v>418</v>
       </c>
     </row>
   </sheetData>
@@ -3399,7 +3405,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3407,26 +3413,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>405</v>
+        <v>407</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>428</v>
+        <v>430</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>429</v>
+        <v>431</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
         <v>230</v>
       </c>
     </row>
@@ -3445,42 +3456,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>432</v>
+        <v>434</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>434</v>
+        <v>436</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>436</v>
+        <v>438</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>438</v>
+        <v>440</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
   </sheetData>
@@ -3498,18 +3509,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>445</v>
+        <v>447</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>447</v>
+        <v>449</v>
       </c>
     </row>
   </sheetData>
@@ -3527,18 +3538,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>453</v>
+        <v>455</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>447</v>
+        <v>449</v>
       </c>
     </row>
   </sheetData>
@@ -3556,18 +3567,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>453</v>
+        <v>455</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>447</v>
+        <v>449</v>
       </c>
     </row>
   </sheetData>
@@ -3585,26 +3596,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>459</v>
+        <v>461</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>461</v>
+        <v>463</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>463</v>
+        <v>465</v>
       </c>
     </row>
   </sheetData>
@@ -4075,18 +4086,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>466</v>
+        <v>468</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>468</v>
+        <v>470</v>
       </c>
     </row>
   </sheetData>
@@ -4104,298 +4115,298 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>473</v>
+        <v>475</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>475</v>
+        <v>477</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>477</v>
+        <v>479</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>479</v>
+        <v>481</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>481</v>
+        <v>483</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>483</v>
+        <v>485</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>485</v>
+        <v>487</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>487</v>
+        <v>489</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>491</v>
+        <v>493</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>493</v>
+        <v>495</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>495</v>
+        <v>497</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>499</v>
+        <v>501</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>501</v>
+        <v>503</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>503</v>
+        <v>505</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>505</v>
+        <v>507</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>507</v>
+        <v>509</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>509</v>
+        <v>511</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>511</v>
+        <v>513</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>513</v>
+        <v>515</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>515</v>
+        <v>517</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>517</v>
+        <v>519</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>519</v>
+        <v>521</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>521</v>
+        <v>523</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>523</v>
+        <v>525</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>525</v>
+        <v>527</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>527</v>
+        <v>529</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>529</v>
+        <v>531</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>531</v>
+        <v>533</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>533</v>
+        <v>535</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>535</v>
+        <v>537</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>545</v>
+        <v>547</v>
       </c>
     </row>
   </sheetData>
@@ -4413,18 +4424,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>548</v>
+        <v>550</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>550</v>
+        <v>552</v>
       </c>
     </row>
     <row r="3">
@@ -4437,130 +4448,130 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>552</v>
+        <v>554</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>554</v>
+        <v>556</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>556</v>
+        <v>558</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>558</v>
+        <v>560</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>560</v>
+        <v>562</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>562</v>
+        <v>564</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>564</v>
+        <v>566</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>529</v>
+        <v>531</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>566</v>
+        <v>568</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>568</v>
+        <v>570</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>570</v>
+        <v>572</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>572</v>
+        <v>574</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>574</v>
+        <v>576</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>576</v>
+        <v>578</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>578</v>
+        <v>580</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>580</v>
+        <v>582</v>
       </c>
     </row>
   </sheetData>
@@ -4601,234 +4612,234 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>586</v>
+        <v>588</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>588</v>
+        <v>590</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>590</v>
+        <v>592</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>592</v>
+        <v>594</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>594</v>
+        <v>596</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>596</v>
+        <v>598</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>598</v>
+        <v>600</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>600</v>
+        <v>602</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>602</v>
+        <v>604</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>604</v>
+        <v>606</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>606</v>
+        <v>608</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>608</v>
+        <v>610</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>610</v>
+        <v>612</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>612</v>
+        <v>614</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>614</v>
+        <v>616</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>616</v>
+        <v>618</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>618</v>
+        <v>620</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>529</v>
+        <v>531</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>620</v>
+        <v>622</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>622</v>
+        <v>624</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>624</v>
+        <v>626</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>626</v>
+        <v>628</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>628</v>
+        <v>630</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>630</v>
+        <v>632</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>632</v>
+        <v>634</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>634</v>
+        <v>636</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>636</v>
+        <v>638</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>638</v>
+        <v>640</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>640</v>
+        <v>642</v>
       </c>
     </row>
   </sheetData>
@@ -4878,18 +4889,18 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>646</v>
+        <v>648</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>648</v>
+        <v>650</v>
       </c>
     </row>
     <row r="7">
@@ -4926,10 +4937,10 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>650</v>
+        <v>652</v>
       </c>
     </row>
   </sheetData>
@@ -4963,10 +4974,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>653</v>
+        <v>655</v>
       </c>
     </row>
     <row r="4">
@@ -4979,18 +4990,18 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>655</v>
+        <v>657</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>529</v>
+        <v>531</v>
       </c>
     </row>
     <row r="7">
@@ -5003,98 +5014,98 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>374</v>
+        <v>376</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>657</v>
+        <v>659</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>659</v>
+        <v>661</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>661</v>
+        <v>663</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>663</v>
+        <v>665</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>665</v>
+        <v>667</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>667</v>
+        <v>669</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>669</v>
+        <v>671</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>671</v>
+        <v>673</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>673</v>
+        <v>675</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>675</v>
+        <v>677</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>677</v>
+        <v>679</v>
       </c>
     </row>
   </sheetData>
@@ -5112,106 +5123,106 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>680</v>
+        <v>682</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>682</v>
+        <v>684</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>525</v>
+        <v>527</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>684</v>
+        <v>686</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>686</v>
+        <v>688</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>688</v>
+        <v>690</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>529</v>
+        <v>531</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>690</v>
+        <v>692</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>692</v>
+        <v>694</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>694</v>
+        <v>696</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>696</v>
+        <v>698</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>698</v>
+        <v>700</v>
       </c>
     </row>
   </sheetData>
@@ -5229,18 +5240,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
   </sheetData>
@@ -5258,242 +5269,242 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>703</v>
+        <v>705</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>705</v>
+        <v>707</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>707</v>
+        <v>709</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>709</v>
+        <v>711</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>711</v>
+        <v>713</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>713</v>
+        <v>715</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>715</v>
+        <v>717</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>717</v>
+        <v>719</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>719</v>
+        <v>721</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>721</v>
+        <v>723</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>723</v>
+        <v>725</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>725</v>
+        <v>727</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>727</v>
+        <v>729</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>729</v>
+        <v>731</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>731</v>
+        <v>733</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>733</v>
+        <v>735</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>735</v>
+        <v>737</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>737</v>
+        <v>739</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>739</v>
+        <v>741</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>741</v>
+        <v>743</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>743</v>
+        <v>745</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>745</v>
+        <v>747</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>529</v>
+        <v>531</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>747</v>
+        <v>749</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>749</v>
+        <v>751</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>751</v>
+        <v>753</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>753</v>
+        <v>755</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>755</v>
+        <v>757</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>757</v>
+        <v>759</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>759</v>
+        <v>761</v>
       </c>
     </row>
   </sheetData>
@@ -5697,16 +5708,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>768</v>
+        <v>770</v>
       </c>
     </row>
     <row r="2">
@@ -5714,13 +5725,13 @@
         <v>106</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>769</v>
+        <v>771</v>
       </c>
     </row>
   </sheetData>
@@ -6030,7 +6041,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B84"/>
+  <dimension ref="A1:B85"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6550,15 +6561,15 @@
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>74</v>
+        <v>350</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>351</v>
+        <v>74</v>
       </c>
       <c r="B66" t="s" s="0">
         <v>352</v>
@@ -6582,18 +6593,18 @@
     </row>
     <row r="69">
       <c r="A69" t="s" s="0">
-        <v>187</v>
+        <v>357</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>188</v>
+        <v>358</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s" s="0">
-        <v>357</v>
+        <v>187</v>
       </c>
       <c r="B70" t="s" s="0">
-        <v>358</v>
+        <v>188</v>
       </c>
     </row>
     <row r="71">
@@ -6706,6 +6717,14 @@
       </c>
       <c r="B84" t="s" s="0">
         <v>386</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s" s="0">
+        <v>387</v>
+      </c>
+      <c r="B85" t="s" s="0">
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -6723,42 +6742,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>392</v>
+        <v>394</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
   </sheetData>
@@ -6776,26 +6795,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>392</v>
+        <v>394</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
   </sheetData>
@@ -6813,42 +6832,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>404</v>
+        <v>406</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>405</v>
+        <v>407</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>406</v>
+        <v>408</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>407</v>
+        <v>409</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>408</v>
+        <v>410</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>409</v>
+        <v>411</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>410</v>
+        <v>412</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="9">

</xml_diff>